<commit_message>
Update inventory processing to generate SKUs in the site's current format
Modify the inventory processing script to always generate new SKUs using the site's format, ignoring existing SKUs from the input file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 81a1a854-4b63-4828-b064-8f991726490e
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: d3208f2d-84c4-4b0d-9317-f1697305fadb
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/6e81966b-af7d-438d-b68d-89d915c5170b/81a1a854-4b63-4828-b064-8f991726490e/bGqtakN
</commit_message>
<xml_diff>
--- a/inventory_import_ready.xlsx
+++ b/inventory_import_ready.xlsx
@@ -444,7 +444,7 @@
   <cols>
     <col width="36" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="21" customWidth="1" min="5" max="5"/>
     <col width="50" customWidth="1" min="6" max="6"/>
@@ -599,7 +599,7 @@
       <c r="B2" s="2" t="inlineStr"/>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>A0000038</t>
+          <t>DB-4X5I</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr"/>
@@ -673,7 +673,7 @@
       <c r="B3" s="2" t="inlineStr"/>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>A0000040</t>
+          <t>DB-MNH</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr"/>
@@ -747,7 +747,7 @@
       <c r="B4" s="2" t="inlineStr"/>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>A0000054</t>
+          <t>DB-XFNH</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr"/>
@@ -821,7 +821,7 @@
       <c r="B5" s="2" t="inlineStr"/>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>A0000061</t>
+          <t>DES-ST5D</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr"/>
@@ -895,7 +895,7 @@
       <c r="B6" s="2" t="inlineStr"/>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>A0000062</t>
+          <t>DES-ST3D</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr"/>
@@ -969,7 +969,7 @@
       <c r="B7" s="2" t="inlineStr"/>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>A0000063</t>
+          <t>DES-ST2D</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr"/>
@@ -1043,7 +1043,7 @@
       <c r="B8" s="2" t="inlineStr"/>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>A0000064</t>
+          <t>DES-FOISTI</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr"/>
@@ -1117,7 +1117,7 @@
       <c r="B9" s="2" t="inlineStr"/>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>A0000066</t>
+          <t>TIP-TINANH</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr"/>
@@ -1191,7 +1191,7 @@
       <c r="B10" s="2" t="inlineStr"/>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>A0000067</t>
+          <t>TIP-TINATH</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr"/>
@@ -1265,7 +1265,7 @@
       <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>A0000068</t>
+          <t>TIP-TINANH-1</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr"/>
@@ -1339,7 +1339,7 @@
       <c r="B12" s="2" t="inlineStr"/>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>A0000070</t>
+          <t>TIP-TITRNH</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr"/>
@@ -1413,7 +1413,7 @@
       <c r="B13" s="2" t="inlineStr"/>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>A0000071</t>
+          <t>DES-DANH7M</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr"/>
@@ -1487,7 +1487,7 @@
       <c r="B14" s="2" t="inlineStr"/>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>A0000073</t>
+          <t>BUT-BUVE1S</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr"/>
@@ -1561,7 +1561,7 @@
       <c r="B15" s="2" t="inlineStr"/>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>A0000075</t>
+          <t>TA-HODUMO</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr"/>
@@ -1635,7 +1635,7 @@
       <c r="B16" s="2" t="inlineStr"/>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>A0000083</t>
+          <t>TA-CAFE</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr"/>
@@ -1709,7 +1709,7 @@
       <c r="B17" s="2" t="inlineStr"/>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>A0000084</t>
+          <t>TA-CAFE-1</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr"/>
@@ -1783,7 +1783,7 @@
       <c r="B18" s="2" t="inlineStr"/>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>A0000096</t>
+          <t>DB-MINFUS</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr"/>
@@ -1857,7 +1857,7 @@
       <c r="B19" s="2" t="inlineStr"/>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>A0000097</t>
+          <t>TA-FREA</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr"/>
@@ -1931,7 +1931,7 @@
       <c r="B20" s="2" t="inlineStr"/>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>A0000098</t>
+          <t>TA-FREB</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr"/>
@@ -2005,7 +2005,7 @@
       <c r="B21" s="2" t="inlineStr"/>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>A0000102</t>
+          <t>DES-STILUA</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr"/>
@@ -2079,7 +2079,7 @@
       <c r="B22" s="2" t="inlineStr"/>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>A0000107</t>
+          <t>BUT-BUVE2</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr"/>
@@ -2153,7 +2153,7 @@
       <c r="B23" s="2" t="inlineStr"/>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>A0000111</t>
+          <t>DES-CHRRED</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr"/>
@@ -2227,7 +2227,7 @@
       <c r="B24" s="2" t="inlineStr"/>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>A0000112</t>
+          <t>HC-SOULBL</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr"/>
@@ -2301,7 +2301,7 @@
       <c r="B25" s="2" t="inlineStr"/>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>A0000113</t>
+          <t>HC-SOULWH</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr"/>
@@ -2375,7 +2375,7 @@
       <c r="B26" s="2" t="inlineStr"/>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>A0000114</t>
+          <t>TA-VONHTI</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr"/>
@@ -2449,7 +2449,7 @@
       <c r="B27" s="2" t="inlineStr"/>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>A0000118</t>
+          <t>BUT-BUTFEN</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr"/>
@@ -2523,7 +2523,7 @@
       <c r="B28" s="2" t="inlineStr"/>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>A0000119</t>
+          <t>BUT-BUTOMB</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr"/>
@@ -2597,7 +2597,7 @@
       <c r="B29" s="2" t="inlineStr"/>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>A0000122</t>
+          <t>TA-VONHTR</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr"/>
@@ -2671,7 +2671,7 @@
       <c r="B30" s="2" t="inlineStr"/>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>A0000124</t>
+          <t>HC-SESOMA</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr"/>
@@ -2745,7 +2745,7 @@
       <c r="B31" s="2" t="inlineStr"/>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>A0000125</t>
+          <t>TA-DAKESO</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr"/>
@@ -2819,7 +2819,7 @@
       <c r="B32" s="2" t="inlineStr"/>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>A0000133</t>
+          <t>DES-STIBUO</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr"/>
@@ -2893,7 +2893,7 @@
       <c r="B33" s="2" t="inlineStr"/>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>A0000134</t>
+          <t>DES-DARA28</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr"/>
@@ -2967,7 +2967,7 @@
       <c r="B34" s="2" t="inlineStr"/>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>A0000135</t>
+          <t>TA-KETASI</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr"/>
@@ -3041,7 +3041,7 @@
       <c r="B35" s="2" t="inlineStr"/>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>A0000137</t>
+          <t>DES-BUMUVE</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr"/>
@@ -3115,7 +3115,7 @@
       <c r="B36" s="2" t="inlineStr"/>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>A0000138</t>
+          <t>DB-5IPH2X</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr"/>
@@ -3189,7 +3189,7 @@
       <c r="B37" s="2" t="inlineStr"/>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>A0000143</t>
+          <t>BUT-BUDAGE</t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr"/>
@@ -3263,7 +3263,7 @@
       <c r="B38" s="2" t="inlineStr"/>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>A0000148</t>
+          <t>TIP-TITHGO</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr"/>
@@ -3333,7 +3333,7 @@
       <c r="B39" s="2" t="inlineStr"/>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>A0000151</t>
+          <t>BUT-BUGEDO</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr"/>
@@ -3407,7 +3407,7 @@
       <c r="B40" s="2" t="inlineStr"/>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>A0000166</t>
+          <t>DES-INFRE</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr"/>
@@ -3481,7 +3481,7 @@
       <c r="B41" s="2" t="inlineStr"/>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>A0000167</t>
+          <t>TA-DACAFE</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr"/>
@@ -3555,7 +3555,7 @@
       <c r="B42" s="2" t="inlineStr"/>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>A0000170</t>
+          <t>DES-STIPLA</t>
         </is>
       </c>
       <c r="D42" s="2" t="inlineStr"/>
@@ -3629,7 +3629,7 @@
       <c r="B43" s="2" t="inlineStr"/>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>A0000173</t>
+          <t>DES-GOLFOI</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr"/>
@@ -3703,7 +3703,7 @@
       <c r="B44" s="2" t="inlineStr"/>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>A0000174</t>
+          <t>BUT-BUGE</t>
         </is>
       </c>
       <c r="D44" s="2" t="inlineStr"/>
@@ -3777,7 +3777,7 @@
       <c r="B45" s="2" t="inlineStr"/>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>A0000175</t>
+          <t>BUT-BUGEQU</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr"/>
@@ -3851,7 +3851,7 @@
       <c r="B46" s="2" t="inlineStr"/>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>A0000178</t>
+          <t>DB-SEBA</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr"/>
@@ -3925,7 +3925,7 @@
       <c r="B47" s="2" t="inlineStr"/>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>A0000188</t>
+          <t>TIP-TIVUTR</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr"/>
@@ -3999,7 +3999,7 @@
       <c r="B48" s="2" t="inlineStr"/>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>A0000189</t>
+          <t>TA-BAMO77</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr"/>
@@ -4073,7 +4073,7 @@
       <c r="B49" s="2" t="inlineStr"/>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>A0000193</t>
+          <t>DES-STHAPH</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr"/>
@@ -4147,7 +4147,7 @@
       <c r="B50" s="2" t="inlineStr"/>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>A0000196</t>
+          <t>HC-TOMA15</t>
         </is>
       </c>
       <c r="D50" s="2" t="inlineStr"/>
@@ -4221,7 +4221,7 @@
       <c r="B51" s="2" t="inlineStr"/>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>A0000197</t>
+          <t>HC-FOIGEL</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr"/>
@@ -4295,7 +4295,7 @@
       <c r="B52" s="2" t="inlineStr"/>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>A0000198</t>
+          <t>DES-STIPLA-1</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr"/>
@@ -4369,7 +4369,7 @@
       <c r="B53" s="2" t="inlineStr"/>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>A0000201</t>
+          <t>TA-BIXIOM</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr"/>
@@ -4443,7 +4443,7 @@
       <c r="B54" s="2" t="inlineStr"/>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>A0000202</t>
+          <t>TA-TAGIME</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr"/>
@@ -4517,7 +4517,7 @@
       <c r="B55" s="2" t="inlineStr"/>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>A0000203</t>
+          <t>TA-TAGIKH</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr"/>
@@ -4591,7 +4591,7 @@
       <c r="B56" s="2" t="inlineStr"/>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>A0000209</t>
+          <t>BUT-BUTGRA</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr"/>
@@ -4665,7 +4665,7 @@
       <c r="B57" s="2" t="inlineStr"/>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>A0000211</t>
+          <t>DB-DACHSA</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr"/>
@@ -4739,7 +4739,7 @@
       <c r="B58" s="2" t="inlineStr"/>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>A0000214</t>
+          <t>DB-3IMIC</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr"/>
@@ -4813,7 +4813,7 @@
       <c r="B59" s="2" t="inlineStr"/>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>A0000219</t>
+          <t>DB-3XCULT</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr"/>
@@ -4887,7 +4887,7 @@
       <c r="B60" s="2" t="inlineStr"/>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>A0000221</t>
+          <t>DB-5XTI</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr"/>
@@ -4961,7 +4961,7 @@
       <c r="B61" s="2" t="inlineStr"/>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>A0000222</t>
+          <t>DB-BANHDI</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr"/>
@@ -5035,7 +5035,7 @@
       <c r="B62" s="2" t="inlineStr"/>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>A0000223</t>
+          <t>DB-BANHDI-1</t>
         </is>
       </c>
       <c r="D62" s="2" t="inlineStr"/>
@@ -5109,7 +5109,7 @@
       <c r="B63" s="2" t="inlineStr"/>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>A0000225</t>
+          <t>DES-HO3DDE</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr"/>
@@ -5183,7 +5183,7 @@
       <c r="B64" s="2" t="inlineStr"/>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>A0000230</t>
+          <t>DES-STICHU</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr"/>
@@ -5257,7 +5257,7 @@
       <c r="B65" s="2" t="inlineStr"/>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>A0000232</t>
+          <t>TIP-TIBATR</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr"/>
@@ -5331,7 +5331,7 @@
       <c r="B66" s="2" t="inlineStr"/>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>A0000233</t>
+          <t>TA-TIBANG</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr"/>
@@ -5405,7 +5405,7 @@
       <c r="B67" s="2" t="inlineStr"/>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>A0000235</t>
+          <t>TA-TITRNH</t>
         </is>
       </c>
       <c r="D67" s="2" t="inlineStr"/>
@@ -5479,7 +5479,7 @@
       <c r="B68" s="2" t="inlineStr"/>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>A0000239</t>
+          <t>DES-LATRTI</t>
         </is>
       </c>
       <c r="D68" s="2" t="inlineStr"/>
@@ -5553,7 +5553,7 @@
       <c r="B69" s="2" t="inlineStr"/>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>A0000250</t>
+          <t>HC-BOMA56</t>
         </is>
       </c>
       <c r="D69" s="2" t="inlineStr"/>
@@ -5627,7 +5627,7 @@
       <c r="B70" s="2" t="inlineStr"/>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>A0000251</t>
+          <t>DD-MAXIOM</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr"/>
@@ -5701,7 +5701,7 @@
       <c r="B71" s="2" t="inlineStr"/>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>A0000252</t>
+          <t>DES-SOVEHU</t>
         </is>
       </c>
       <c r="D71" s="2" t="inlineStr"/>
@@ -5775,7 +5775,7 @@
       <c r="B72" s="2" t="inlineStr"/>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>A0000253</t>
+          <t>DES-SOVEHU-1</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr"/>
@@ -5849,7 +5849,7 @@
       <c r="B73" s="2" t="inlineStr"/>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>A0000254</t>
+          <t>HC-CUOI15</t>
         </is>
       </c>
       <c r="D73" s="2" t="inlineStr"/>
@@ -5923,7 +5923,7 @@
       <c r="B74" s="2" t="inlineStr"/>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>A0000256</t>
+          <t>DES-GEVEMA</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr"/>
@@ -5997,7 +5997,7 @@
       <c r="B75" s="2" t="inlineStr"/>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>A0000258</t>
+          <t>TA-NHTRM</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr"/>
@@ -6071,7 +6071,7 @@
       <c r="B76" s="2" t="inlineStr"/>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>A0000259</t>
+          <t>TIP-TITRNH-1</t>
         </is>
       </c>
       <c r="D76" s="2" t="inlineStr"/>
@@ -6145,7 +6145,7 @@
       <c r="B77" s="2" t="inlineStr"/>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>A0000260</t>
+          <t>TIP-LETI</t>
         </is>
       </c>
       <c r="D77" s="2" t="inlineStr"/>
@@ -6219,7 +6219,7 @@
       <c r="B78" s="2" t="inlineStr"/>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>A0000261</t>
+          <t>DB-BADICU</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr"/>
@@ -6293,7 +6293,7 @@
       <c r="B79" s="2" t="inlineStr"/>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>A0000262</t>
+          <t>DES-STFNO</t>
         </is>
       </c>
       <c r="D79" s="2" t="inlineStr"/>
@@ -6367,7 +6367,7 @@
       <c r="B80" s="2" t="inlineStr"/>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>A0000263</t>
+          <t>DES-STSTNO</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr"/>
@@ -6441,7 +6441,7 @@
       <c r="B81" s="2" t="inlineStr"/>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>A0000266</t>
+          <t>TA-KEO</t>
         </is>
       </c>
       <c r="D81" s="2" t="inlineStr"/>
@@ -6515,7 +6515,7 @@
       <c r="B82" s="2" t="inlineStr"/>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>A0000267</t>
+          <t>DD-MABABT</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr"/>
@@ -6589,7 +6589,7 @@
       <c r="B83" s="2" t="inlineStr"/>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>A0000268</t>
+          <t>TA-BUCHBI</t>
         </is>
       </c>
       <c r="D83" s="2" t="inlineStr"/>
@@ -6663,7 +6663,7 @@
       <c r="B84" s="2" t="inlineStr"/>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>A0000270</t>
+          <t>TA-CADACA</t>
         </is>
       </c>
       <c r="D84" s="2" t="inlineStr"/>
@@ -6737,7 +6737,7 @@
       <c r="B85" s="2" t="inlineStr"/>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>A0000271</t>
+          <t>DD-DELEPI</t>
         </is>
       </c>
       <c r="D85" s="2" t="inlineStr"/>
@@ -6811,7 +6811,7 @@
       <c r="B86" s="2" t="inlineStr"/>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>A0000272</t>
+          <t>TA-KHAINO</t>
         </is>
       </c>
       <c r="D86" s="2" t="inlineStr"/>
@@ -6885,7 +6885,7 @@
       <c r="B87" s="2" t="inlineStr"/>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>A0001032</t>
+          <t>DD-TATHMA</t>
         </is>
       </c>
       <c r="D87" s="2" t="inlineStr"/>
@@ -6959,7 +6959,7 @@
       <c r="B88" s="2" t="inlineStr"/>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>A0000276</t>
+          <t>TA-CADADA</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr"/>
@@ -7033,7 +7033,7 @@
       <c r="B89" s="2" t="inlineStr"/>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>A0000277</t>
+          <t>DB-3XHOCU</t>
         </is>
       </c>
       <c r="D89" s="2" t="inlineStr"/>
@@ -7107,7 +7107,7 @@
       <c r="B90" s="2" t="inlineStr"/>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>A0000278</t>
+          <t>BUT-BUQUTA</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr"/>
@@ -7181,7 +7181,7 @@
       <c r="B91" s="2" t="inlineStr"/>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>A0000281</t>
+          <t>BUT-BUVE2-1</t>
         </is>
       </c>
       <c r="D91" s="2" t="inlineStr"/>
@@ -7255,7 +7255,7 @@
       <c r="B92" s="2" t="inlineStr"/>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>A0000282</t>
+          <t>TA-KEDA</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr"/>
@@ -7329,7 +7329,7 @@
       <c r="B93" s="2" t="inlineStr"/>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>A0000287</t>
+          <t>DB-4XTI</t>
         </is>
       </c>
       <c r="D93" s="2" t="inlineStr"/>
@@ -7403,7 +7403,7 @@
       <c r="B94" s="2" t="inlineStr"/>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>A0000290</t>
+          <t>DB-4XTRNH</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr"/>
@@ -7477,7 +7477,7 @@
       <c r="B95" s="2" t="inlineStr"/>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>A0000291</t>
+          <t>TA-VONHTR-1</t>
         </is>
       </c>
       <c r="D95" s="2" t="inlineStr"/>
@@ -7551,7 +7551,7 @@
       <c r="B96" s="2" t="inlineStr"/>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t>A0000292</t>
+          <t>TA-GATALA</t>
         </is>
       </c>
       <c r="D96" s="2" t="inlineStr"/>
@@ -7625,7 +7625,7 @@
       <c r="B97" s="2" t="inlineStr"/>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>A0000293</t>
+          <t>TA-GATALA-1</t>
         </is>
       </c>
       <c r="D97" s="2" t="inlineStr"/>
@@ -7699,7 +7699,7 @@
       <c r="B98" s="2" t="inlineStr"/>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>A0000296</t>
+          <t>TA-CHCH2</t>
         </is>
       </c>
       <c r="D98" s="2" t="inlineStr"/>
@@ -7773,7 +7773,7 @@
       <c r="B99" s="2" t="inlineStr"/>
       <c r="C99" s="2" t="inlineStr">
         <is>
-          <t>A0000299</t>
+          <t>HC-NURUCO</t>
         </is>
       </c>
       <c r="D99" s="2" t="inlineStr"/>
@@ -7847,7 +7847,7 @@
       <c r="B100" s="2" t="inlineStr"/>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>A0001180</t>
+          <t>DB-BAOGAM</t>
         </is>
       </c>
       <c r="D100" s="2" t="inlineStr"/>
@@ -7921,7 +7921,7 @@
       <c r="B101" s="2" t="inlineStr"/>
       <c r="C101" s="2" t="inlineStr">
         <is>
-          <t>A0000309</t>
+          <t>HC-GEDIDA</t>
         </is>
       </c>
       <c r="D101" s="2" t="inlineStr"/>
@@ -7995,7 +7995,7 @@
       <c r="B102" s="2" t="inlineStr"/>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>A0000317</t>
+          <t>HC-BNSKEO</t>
         </is>
       </c>
       <c r="D102" s="2" t="inlineStr"/>
@@ -8069,7 +8069,7 @@
       <c r="B103" s="2" t="inlineStr"/>
       <c r="C103" s="2" t="inlineStr">
         <is>
-          <t>A0000326</t>
+          <t>TC-15TOCO</t>
         </is>
       </c>
       <c r="D103" s="2" t="inlineStr"/>
@@ -8143,7 +8143,7 @@
       <c r="B104" s="2" t="inlineStr"/>
       <c r="C104" s="2" t="inlineStr">
         <is>
-          <t>A0000347</t>
+          <t>TIP-TITRVU</t>
         </is>
       </c>
       <c r="D104" s="2" t="inlineStr"/>
@@ -8217,7 +8217,7 @@
       <c r="B105" s="2" t="inlineStr"/>
       <c r="C105" s="2" t="inlineStr">
         <is>
-          <t>A0000352</t>
+          <t>TA-CHPHBA</t>
         </is>
       </c>
       <c r="D105" s="2" t="inlineStr"/>
@@ -8291,7 +8291,7 @@
       <c r="B106" s="2" t="inlineStr"/>
       <c r="C106" s="2" t="inlineStr">
         <is>
-          <t>A0000354</t>
+          <t>HC-SPTA2G</t>
         </is>
       </c>
       <c r="D106" s="2" t="inlineStr"/>
@@ -8365,7 +8365,7 @@
       <c r="B107" s="2" t="inlineStr"/>
       <c r="C107" s="2" t="inlineStr">
         <is>
-          <t>A0000356</t>
+          <t>DES-NHUDUO</t>
         </is>
       </c>
       <c r="D107" s="2" t="inlineStr"/>
@@ -8439,7 +8439,7 @@
       <c r="B108" s="2" t="inlineStr"/>
       <c r="C108" s="2" t="inlineStr">
         <is>
-          <t>A0000365</t>
+          <t>BUT-BUQUTA-1</t>
         </is>
       </c>
       <c r="D108" s="2" t="inlineStr"/>
@@ -8513,7 +8513,7 @@
       <c r="B109" s="2" t="inlineStr"/>
       <c r="C109" s="2" t="inlineStr">
         <is>
-          <t>A0000370</t>
+          <t>BUT-BUGE-1</t>
         </is>
       </c>
       <c r="D109" s="2" t="inlineStr"/>
@@ -8587,7 +8587,7 @@
       <c r="B110" s="2" t="inlineStr"/>
       <c r="C110" s="2" t="inlineStr">
         <is>
-          <t>A0000375</t>
+          <t>DD-SUBAKO</t>
         </is>
       </c>
       <c r="D110" s="2" t="inlineStr"/>
@@ -8661,7 +8661,7 @@
       <c r="B111" s="2" t="inlineStr"/>
       <c r="C111" s="2" t="inlineStr">
         <is>
-          <t>A0000380</t>
+          <t>DB-XC</t>
         </is>
       </c>
       <c r="D111" s="2" t="inlineStr"/>
@@ -8735,7 +8735,7 @@
       <c r="B112" s="2" t="inlineStr"/>
       <c r="C112" s="2" t="inlineStr">
         <is>
-          <t>A0000383</t>
+          <t>TA-BANGCA</t>
         </is>
       </c>
       <c r="D112" s="2" t="inlineStr"/>
@@ -8809,7 +8809,7 @@
       <c r="B113" s="2" t="inlineStr"/>
       <c r="C113" s="2" t="inlineStr">
         <is>
-          <t>A0000393</t>
+          <t>TC-TOCO50</t>
         </is>
       </c>
       <c r="D113" s="2" t="inlineStr"/>
@@ -8883,7 +8883,7 @@
       <c r="B114" s="2" t="inlineStr"/>
       <c r="C114" s="2" t="inlineStr">
         <is>
-          <t>A0001062</t>
+          <t>DES-CHTRGU</t>
         </is>
       </c>
       <c r="D114" s="2" t="inlineStr"/>
@@ -8957,7 +8957,7 @@
       <c r="B115" s="2" t="inlineStr"/>
       <c r="C115" s="2" t="inlineStr">
         <is>
-          <t>A0000395</t>
+          <t>HC-TOMA25</t>
         </is>
       </c>
       <c r="D115" s="2" t="inlineStr"/>
@@ -9031,7 +9031,7 @@
       <c r="B116" s="2" t="inlineStr"/>
       <c r="C116" s="2" t="inlineStr">
         <is>
-          <t>A0000402</t>
+          <t>TA-CHCH1</t>
         </is>
       </c>
       <c r="D116" s="2" t="inlineStr"/>
@@ -9105,7 +9105,7 @@
       <c r="B117" s="2" t="inlineStr"/>
       <c r="C117" s="2" t="inlineStr">
         <is>
-          <t>A0000407</t>
+          <t>DB-BAMIDI</t>
         </is>
       </c>
       <c r="D117" s="2" t="inlineStr"/>
@@ -9179,7 +9179,7 @@
       <c r="B118" s="2" t="inlineStr"/>
       <c r="C118" s="2" t="inlineStr">
         <is>
-          <t>A0000412</t>
+          <t>DB-MIFU</t>
         </is>
       </c>
       <c r="D118" s="2" t="inlineStr"/>
@@ -9253,7 +9253,7 @@
       <c r="B119" s="2" t="inlineStr"/>
       <c r="C119" s="2" t="inlineStr">
         <is>
-          <t>A0000413</t>
+          <t>DB-MIFU-1</t>
         </is>
       </c>
       <c r="D119" s="2" t="inlineStr"/>
@@ -9327,7 +9327,7 @@
       <c r="B120" s="2" t="inlineStr"/>
       <c r="C120" s="2" t="inlineStr">
         <is>
-          <t>A0000414</t>
+          <t>DB-3XRATH</t>
         </is>
       </c>
       <c r="D120" s="2" t="inlineStr"/>
@@ -9401,7 +9401,7 @@
       <c r="B121" s="2" t="inlineStr"/>
       <c r="C121" s="2" t="inlineStr">
         <is>
-          <t>A0000415</t>
+          <t>DB-4XRATH</t>
         </is>
       </c>
       <c r="D121" s="2" t="inlineStr"/>
@@ -9475,7 +9475,7 @@
       <c r="B122" s="2" t="inlineStr"/>
       <c r="C122" s="2" t="inlineStr">
         <is>
-          <t>A0000416</t>
+          <t>DB-TRNHRE</t>
         </is>
       </c>
       <c r="D122" s="2" t="inlineStr"/>
@@ -9549,7 +9549,7 @@
       <c r="B123" s="2" t="inlineStr"/>
       <c r="C123" s="2" t="inlineStr">
         <is>
-          <t>A0000420</t>
+          <t>BUT-BUCAGO</t>
         </is>
       </c>
       <c r="D123" s="2" t="inlineStr"/>
@@ -9623,7 +9623,7 @@
       <c r="B124" s="2" t="inlineStr"/>
       <c r="C124" s="2" t="inlineStr">
         <is>
-          <t>A0000434</t>
+          <t>DES-CHLI</t>
         </is>
       </c>
       <c r="D124" s="2" t="inlineStr"/>
@@ -9697,7 +9697,7 @@
       <c r="B125" s="2" t="inlineStr"/>
       <c r="C125" s="2" t="inlineStr">
         <is>
-          <t>A0000989</t>
+          <t>HC-BACO25</t>
         </is>
       </c>
       <c r="D125" s="2" t="inlineStr"/>
@@ -9771,7 +9771,7 @@
       <c r="B126" s="2" t="inlineStr"/>
       <c r="C126" s="2" t="inlineStr">
         <is>
-          <t>A0001104</t>
+          <t>HC-TOLO</t>
         </is>
       </c>
       <c r="D126" s="2" t="inlineStr"/>
@@ -9845,7 +9845,7 @@
       <c r="B127" s="2" t="inlineStr"/>
       <c r="C127" s="2" t="inlineStr">
         <is>
-          <t>A0000457</t>
+          <t>TA-5IPEKI</t>
         </is>
       </c>
       <c r="D127" s="2" t="inlineStr"/>
@@ -9919,7 +9919,7 @@
       <c r="B128" s="2" t="inlineStr"/>
       <c r="C128" s="2" t="inlineStr">
         <is>
-          <t>A0000460</t>
+          <t>TA-BUDECA</t>
         </is>
       </c>
       <c r="D128" s="2" t="inlineStr"/>
@@ -9993,7 +9993,7 @@
       <c r="B129" s="2" t="inlineStr"/>
       <c r="C129" s="2" t="inlineStr">
         <is>
-          <t>A0000464</t>
+          <t>TIP-TIBA</t>
         </is>
       </c>
       <c r="D129" s="2" t="inlineStr"/>
@@ -10067,7 +10067,7 @@
       <c r="B130" s="2" t="inlineStr"/>
       <c r="C130" s="2" t="inlineStr">
         <is>
-          <t>A0000466</t>
+          <t>DES-KITUDL</t>
         </is>
       </c>
       <c r="D130" s="2" t="inlineStr"/>
@@ -10141,7 +10141,7 @@
       <c r="B131" s="2" t="inlineStr"/>
       <c r="C131" s="2" t="inlineStr">
         <is>
-          <t>A0000467</t>
+          <t>DES-KITUDL-1</t>
         </is>
       </c>
       <c r="D131" s="2" t="inlineStr"/>
@@ -10215,7 +10215,7 @@
       <c r="B132" s="2" t="inlineStr"/>
       <c r="C132" s="2" t="inlineStr">
         <is>
-          <t>A0000468</t>
+          <t>DES-KITUSA</t>
         </is>
       </c>
       <c r="D132" s="2" t="inlineStr"/>
@@ -10289,7 +10289,7 @@
       <c r="B133" s="2" t="inlineStr"/>
       <c r="C133" s="2" t="inlineStr">
         <is>
-          <t>A0000470</t>
+          <t>TA-COCLIQ</t>
         </is>
       </c>
       <c r="D133" s="2" t="inlineStr"/>
@@ -10363,7 +10363,7 @@
       <c r="B134" s="2" t="inlineStr"/>
       <c r="C134" s="2" t="inlineStr">
         <is>
-          <t>A0000471</t>
+          <t>DB-XXDA</t>
         </is>
       </c>
       <c r="D134" s="2" t="inlineStr"/>
@@ -10437,7 +10437,7 @@
       <c r="B135" s="2" t="inlineStr"/>
       <c r="C135" s="2" t="inlineStr">
         <is>
-          <t>A0000473</t>
+          <t>DB-BAVIDA</t>
         </is>
       </c>
       <c r="D135" s="2" t="inlineStr"/>
@@ -10511,7 +10511,7 @@
       <c r="B136" s="2" t="inlineStr"/>
       <c r="C136" s="2" t="inlineStr">
         <is>
-          <t>A0000478</t>
+          <t>DB-4XDATR</t>
         </is>
       </c>
       <c r="D136" s="2" t="inlineStr"/>
@@ -10585,7 +10585,7 @@
       <c r="B137" s="2" t="inlineStr"/>
       <c r="C137" s="2" t="inlineStr">
         <is>
-          <t>A0001050</t>
+          <t>TA-CADACA-1</t>
         </is>
       </c>
       <c r="D137" s="2" t="inlineStr"/>
@@ -10659,7 +10659,7 @@
       <c r="B138" s="2" t="inlineStr"/>
       <c r="C138" s="2" t="inlineStr">
         <is>
-          <t>A0000480</t>
+          <t>DES-NHDU</t>
         </is>
       </c>
       <c r="D138" s="2" t="inlineStr"/>
@@ -10733,7 +10733,7 @@
       <c r="B139" s="2" t="inlineStr"/>
       <c r="C139" s="2" t="inlineStr">
         <is>
-          <t>A0000482</t>
+          <t>HC-KEMEDA</t>
         </is>
       </c>
       <c r="D139" s="2" t="inlineStr"/>
@@ -10807,7 +10807,7 @@
       <c r="B140" s="2" t="inlineStr"/>
       <c r="C140" s="2" t="inlineStr">
         <is>
-          <t>A0000483</t>
+          <t>HC-LIQMAN</t>
         </is>
       </c>
       <c r="D140" s="2" t="inlineStr"/>
@@ -10881,7 +10881,7 @@
       <c r="B141" s="2" t="inlineStr"/>
       <c r="C141" s="2" t="inlineStr">
         <is>
-          <t>A0000494</t>
+          <t>TA-VONHMI</t>
         </is>
       </c>
       <c r="D141" s="2" t="inlineStr"/>
@@ -10955,7 +10955,7 @@
       <c r="B142" s="2" t="inlineStr"/>
       <c r="C142" s="2" t="inlineStr">
         <is>
-          <t>A0000495</t>
+          <t>TA-VONHMI-1</t>
         </is>
       </c>
       <c r="D142" s="2" t="inlineStr"/>
@@ -11029,7 +11029,7 @@
       <c r="B143" s="2" t="inlineStr"/>
       <c r="C143" s="2" t="inlineStr">
         <is>
-          <t>A0000497</t>
+          <t>TA-VONHTR-2</t>
         </is>
       </c>
       <c r="D143" s="2" t="inlineStr"/>
@@ -11103,7 +11103,7 @@
       <c r="B144" s="2" t="inlineStr"/>
       <c r="C144" s="2" t="inlineStr">
         <is>
-          <t>A0000504</t>
+          <t>DD-SUBAMA</t>
         </is>
       </c>
       <c r="D144" s="2" t="inlineStr"/>
@@ -11177,7 +11177,7 @@
       <c r="B145" s="2" t="inlineStr"/>
       <c r="C145" s="2" t="inlineStr">
         <is>
-          <t>A0000506</t>
+          <t>DD-VOBIDU</t>
         </is>
       </c>
       <c r="D145" s="2" t="inlineStr"/>
@@ -11251,7 +11251,7 @@
       <c r="B146" s="2" t="inlineStr"/>
       <c r="C146" s="2" t="inlineStr">
         <is>
-          <t>A0000507</t>
+          <t>DD-VOBIDU-1</t>
         </is>
       </c>
       <c r="D146" s="2" t="inlineStr"/>
@@ -11325,7 +11325,7 @@
       <c r="B147" s="2" t="inlineStr"/>
       <c r="C147" s="2" t="inlineStr">
         <is>
-          <t>A0000511</t>
+          <t>BOT-BONA</t>
         </is>
       </c>
       <c r="D147" s="2" t="inlineStr"/>
@@ -11399,7 +11399,7 @@
       <c r="B148" s="2" t="inlineStr"/>
       <c r="C148" s="2" t="inlineStr">
         <is>
-          <t>A0001007</t>
+          <t>HC-XOGESC</t>
         </is>
       </c>
       <c r="D148" s="2" t="inlineStr"/>
@@ -11473,7 +11473,7 @@
       <c r="B149" s="2" t="inlineStr"/>
       <c r="C149" s="2" t="inlineStr">
         <is>
-          <t>A0000516</t>
+          <t>HC-CUOI</t>
         </is>
       </c>
       <c r="D149" s="2" t="inlineStr"/>
@@ -11547,7 +11547,7 @@
       <c r="B150" s="2" t="inlineStr"/>
       <c r="C150" s="2" t="inlineStr">
         <is>
-          <t>A0000519</t>
+          <t>TC-TOCOTI</t>
         </is>
       </c>
       <c r="D150" s="2" t="inlineStr"/>
@@ -11621,7 +11621,7 @@
       <c r="B151" s="2" t="inlineStr"/>
       <c r="C151" s="2" t="inlineStr">
         <is>
-          <t>A0000520</t>
+          <t>TC-TOCOTI-1</t>
         </is>
       </c>
       <c r="D151" s="2" t="inlineStr"/>
@@ -11695,7 +11695,7 @@
       <c r="B152" s="2" t="inlineStr"/>
       <c r="C152" s="2" t="inlineStr">
         <is>
-          <t>A0000523</t>
+          <t>BOT-COACPO</t>
         </is>
       </c>
       <c r="D152" s="2" t="inlineStr"/>
@@ -11769,7 +11769,7 @@
       <c r="B153" s="2" t="inlineStr"/>
       <c r="C153" s="2" t="inlineStr">
         <is>
-          <t>A0000524</t>
+          <t>DD-TABATR</t>
         </is>
       </c>
       <c r="D153" s="2" t="inlineStr"/>
@@ -11843,7 +11843,7 @@
       <c r="B154" s="2" t="inlineStr"/>
       <c r="C154" s="2" t="inlineStr">
         <is>
-          <t>A0000525</t>
+          <t>DD-SUTABA</t>
         </is>
       </c>
       <c r="D154" s="2" t="inlineStr"/>
@@ -11917,7 +11917,7 @@
       <c r="B155" s="2" t="inlineStr"/>
       <c r="C155" s="2" t="inlineStr">
         <is>
-          <t>A0000526</t>
+          <t>DD-MABAKO</t>
         </is>
       </c>
       <c r="D155" s="2" t="inlineStr"/>
@@ -11991,7 +11991,7 @@
       <c r="B156" s="2" t="inlineStr"/>
       <c r="C156" s="2" t="inlineStr">
         <is>
-          <t>A0000528</t>
+          <t>TA-TILAMA</t>
         </is>
       </c>
       <c r="D156" s="2" t="inlineStr"/>
@@ -12065,7 +12065,7 @@
       <c r="B157" s="2" t="inlineStr"/>
       <c r="C157" s="2" t="inlineStr">
         <is>
-          <t>A0000531</t>
+          <t>TA-TACABA</t>
         </is>
       </c>
       <c r="D157" s="2" t="inlineStr"/>
@@ -12139,7 +12139,7 @@
       <c r="B158" s="2" t="inlineStr"/>
       <c r="C158" s="2" t="inlineStr">
         <is>
-          <t>A0000533</t>
+          <t>DUA-DUNHPR</t>
         </is>
       </c>
       <c r="D158" s="2" t="inlineStr"/>
@@ -12213,7 +12213,7 @@
       <c r="B159" s="2" t="inlineStr"/>
       <c r="C159" s="2" t="inlineStr">
         <is>
-          <t>A0000543</t>
+          <t>TIP-TINABA</t>
         </is>
       </c>
       <c r="D159" s="2" t="inlineStr"/>
@@ -12287,7 +12287,7 @@
       <c r="B160" s="2" t="inlineStr"/>
       <c r="C160" s="2" t="inlineStr">
         <is>
-          <t>A0000549</t>
+          <t>DD-LOSUG5</t>
         </is>
       </c>
       <c r="D160" s="2" t="inlineStr"/>
@@ -12361,7 +12361,7 @@
       <c r="B161" s="2" t="inlineStr"/>
       <c r="C161" s="2" t="inlineStr">
         <is>
-          <t>A0000551</t>
+          <t>DD-DATAMA</t>
         </is>
       </c>
       <c r="D161" s="2" t="inlineStr"/>
@@ -12435,7 +12435,7 @@
       <c r="B162" s="2" t="inlineStr"/>
       <c r="C162" s="2" t="inlineStr">
         <is>
-          <t>A0001134</t>
+          <t>BOT-BOIN</t>
         </is>
       </c>
       <c r="D162" s="2" t="inlineStr"/>
@@ -12509,7 +12509,7 @@
       <c r="B163" s="2" t="inlineStr"/>
       <c r="C163" s="2" t="inlineStr">
         <is>
-          <t>A0001156</t>
+          <t>BUT-BUDAHO</t>
         </is>
       </c>
       <c r="D163" s="2" t="inlineStr"/>
@@ -12583,7 +12583,7 @@
       <c r="B164" s="2" t="inlineStr"/>
       <c r="C164" s="2" t="inlineStr">
         <is>
-          <t>A0001157</t>
+          <t>BUT-BUDABO</t>
         </is>
       </c>
       <c r="D164" s="2" t="inlineStr"/>
@@ -12657,7 +12657,7 @@
       <c r="B165" s="2" t="inlineStr"/>
       <c r="C165" s="2" t="inlineStr">
         <is>
-          <t>A0000572</t>
+          <t>BUT-CHRANH</t>
         </is>
       </c>
       <c r="D165" s="2" t="inlineStr"/>
@@ -12731,7 +12731,7 @@
       <c r="B166" s="2" t="inlineStr"/>
       <c r="C166" s="2" t="inlineStr">
         <is>
-          <t>A0000573</t>
+          <t>BUT-BUVECO</t>
         </is>
       </c>
       <c r="D166" s="2" t="inlineStr"/>
@@ -12805,7 +12805,7 @@
       <c r="B167" s="2" t="inlineStr"/>
       <c r="C167" s="2" t="inlineStr">
         <is>
-          <t>A0000574</t>
+          <t>BUT-BUVEHO</t>
         </is>
       </c>
       <c r="D167" s="2" t="inlineStr"/>
@@ -12879,7 +12879,7 @@
       <c r="B168" s="2" t="inlineStr"/>
       <c r="C168" s="2" t="inlineStr">
         <is>
-          <t>A0000582</t>
+          <t>DD-DACAO</t>
         </is>
       </c>
       <c r="D168" s="2" t="inlineStr"/>
@@ -12953,7 +12953,7 @@
       <c r="B169" s="2" t="inlineStr"/>
       <c r="C169" s="2" t="inlineStr">
         <is>
-          <t>A0000583</t>
+          <t>DB-MITHXF</t>
         </is>
       </c>
       <c r="D169" s="2" t="inlineStr"/>
@@ -13027,7 +13027,7 @@
       <c r="B170" s="2" t="inlineStr"/>
       <c r="C170" s="2" t="inlineStr">
         <is>
-          <t>A0000586</t>
+          <t>DB-5IPHVO</t>
         </is>
       </c>
       <c r="D170" s="2" t="inlineStr"/>
@@ -13101,7 +13101,7 @@
       <c r="B171" s="2" t="inlineStr"/>
       <c r="C171" s="2" t="inlineStr">
         <is>
-          <t>A0000588</t>
+          <t>DB-5XC</t>
         </is>
       </c>
       <c r="D171" s="2" t="inlineStr"/>
@@ -13175,7 +13175,7 @@
       <c r="B172" s="2" t="inlineStr"/>
       <c r="C172" s="2" t="inlineStr">
         <is>
-          <t>A0000590</t>
+          <t>DB-XXDAVA</t>
         </is>
       </c>
       <c r="D172" s="2" t="inlineStr"/>
@@ -13249,7 +13249,7 @@
       <c r="B173" s="2" t="inlineStr"/>
       <c r="C173" s="2" t="inlineStr">
         <is>
-          <t>A0000592</t>
+          <t>TA-BIGORE</t>
         </is>
       </c>
       <c r="D173" s="2" t="inlineStr"/>
@@ -13323,7 +13323,7 @@
       <c r="B174" s="2" t="inlineStr"/>
       <c r="C174" s="2" t="inlineStr">
         <is>
-          <t>A0000593</t>
+          <t>TA-TRNHMI</t>
         </is>
       </c>
       <c r="D174" s="2" t="inlineStr"/>
@@ -13397,7 +13397,7 @@
       <c r="B175" s="2" t="inlineStr"/>
       <c r="C175" s="2" t="inlineStr">
         <is>
-          <t>A0000594</t>
+          <t>BUT-BUGE-2</t>
         </is>
       </c>
       <c r="D175" s="2" t="inlineStr"/>
@@ -13471,7 +13471,7 @@
       <c r="B176" s="2" t="inlineStr"/>
       <c r="C176" s="2" t="inlineStr">
         <is>
-          <t>A0000595</t>
+          <t>BUT-BUGEQU-1</t>
         </is>
       </c>
       <c r="D176" s="2" t="inlineStr"/>
@@ -13545,7 +13545,7 @@
       <c r="B177" s="2" t="inlineStr"/>
       <c r="C177" s="2" t="inlineStr">
         <is>
-          <t>A0001034</t>
+          <t>HC-KEDNPR</t>
         </is>
       </c>
       <c r="D177" s="2" t="inlineStr"/>
@@ -13619,7 +13619,7 @@
       <c r="B178" s="2" t="inlineStr"/>
       <c r="C178" s="2" t="inlineStr">
         <is>
-          <t>A0000601</t>
+          <t>HC-ULRE5L</t>
         </is>
       </c>
       <c r="D178" s="2" t="inlineStr"/>
@@ -13693,7 +13693,7 @@
       <c r="B179" s="2" t="inlineStr"/>
       <c r="C179" s="2" t="inlineStr">
         <is>
-          <t>A0001027</t>
+          <t>TA-KINGD5</t>
         </is>
       </c>
       <c r="D179" s="2" t="inlineStr"/>
@@ -13767,7 +13767,7 @@
       <c r="B180" s="2" t="inlineStr"/>
       <c r="C180" s="2" t="inlineStr">
         <is>
-          <t>A0001092</t>
+          <t>GD-50GE</t>
         </is>
       </c>
       <c r="D180" s="2" t="inlineStr"/>
@@ -13841,7 +13841,7 @@
       <c r="B181" s="2" t="inlineStr"/>
       <c r="C181" s="2" t="inlineStr">
         <is>
-          <t>A0001105</t>
+          <t>TC-CHBACO</t>
         </is>
       </c>
       <c r="D181" s="2" t="inlineStr"/>
@@ -13915,7 +13915,7 @@
       <c r="B182" s="2" t="inlineStr"/>
       <c r="C182" s="2" t="inlineStr">
         <is>
-          <t>A0001054</t>
+          <t>TA-NACHMA</t>
         </is>
       </c>
       <c r="D182" s="2" t="inlineStr"/>
@@ -13989,7 +13989,7 @@
       <c r="B183" s="2" t="inlineStr"/>
       <c r="C183" s="2" t="inlineStr">
         <is>
-          <t>A0001031</t>
+          <t>DES-CHNGTR</t>
         </is>
       </c>
       <c r="D183" s="2" t="inlineStr"/>
@@ -14063,7 +14063,7 @@
       <c r="B184" s="2" t="inlineStr"/>
       <c r="C184" s="2" t="inlineStr">
         <is>
-          <t>A0000618</t>
+          <t>DES-NHDUD</t>
         </is>
       </c>
       <c r="D184" s="2" t="inlineStr"/>
@@ -14137,7 +14137,7 @@
       <c r="B185" s="2" t="inlineStr"/>
       <c r="C185" s="2" t="inlineStr">
         <is>
-          <t>A0000622</t>
+          <t>TC-15TOCO-1</t>
         </is>
       </c>
       <c r="D185" s="2" t="inlineStr"/>
@@ -14211,7 +14211,7 @@
       <c r="B186" s="2" t="inlineStr"/>
       <c r="C186" s="2" t="inlineStr">
         <is>
-          <t>A0000623</t>
+          <t>TA-KHTRY</t>
         </is>
       </c>
       <c r="D186" s="2" t="inlineStr"/>
@@ -14285,7 +14285,7 @@
       <c r="B187" s="2" t="inlineStr"/>
       <c r="C187" s="2" t="inlineStr">
         <is>
-          <t>A0000624</t>
+          <t>DB-BANAGA</t>
         </is>
       </c>
       <c r="D187" s="2" t="inlineStr"/>
@@ -14359,7 +14359,7 @@
       <c r="B188" s="2" t="inlineStr"/>
       <c r="C188" s="2" t="inlineStr">
         <is>
-          <t>A0001017</t>
+          <t>DB-4XDA</t>
         </is>
       </c>
       <c r="D188" s="2" t="inlineStr"/>
@@ -14433,7 +14433,7 @@
       <c r="B189" s="2" t="inlineStr"/>
       <c r="C189" s="2" t="inlineStr">
         <is>
-          <t>A0001016</t>
+          <t>DB-3IMIC-1</t>
         </is>
       </c>
       <c r="D189" s="2" t="inlineStr"/>
@@ -14507,7 +14507,7 @@
       <c r="B190" s="2" t="inlineStr"/>
       <c r="C190" s="2" t="inlineStr">
         <is>
-          <t>A0001053</t>
+          <t>BUT-BUDABO-1</t>
         </is>
       </c>
       <c r="D190" s="2" t="inlineStr"/>
@@ -14581,7 +14581,7 @@
       <c r="B191" s="2" t="inlineStr"/>
       <c r="C191" s="2" t="inlineStr">
         <is>
-          <t>A0000641</t>
+          <t>TA-NHDOMA</t>
         </is>
       </c>
       <c r="D191" s="2" t="inlineStr"/>
@@ -14655,7 +14655,7 @@
       <c r="B192" s="2" t="inlineStr"/>
       <c r="C192" s="2" t="inlineStr">
         <is>
-          <t>A0000645</t>
+          <t>DD-MABAMA</t>
         </is>
       </c>
       <c r="D192" s="2" t="inlineStr"/>
@@ -14729,7 +14729,7 @@
       <c r="B193" s="2" t="inlineStr"/>
       <c r="C193" s="2" t="inlineStr">
         <is>
-          <t>A0000646</t>
+          <t>DD-DACA3</t>
         </is>
       </c>
       <c r="D193" s="2" t="inlineStr"/>
@@ -14803,7 +14803,7 @@
       <c r="B194" s="2" t="inlineStr"/>
       <c r="C194" s="2" t="inlineStr">
         <is>
-          <t>A0000648</t>
+          <t>DD-DEBALE</t>
         </is>
       </c>
       <c r="D194" s="2" t="inlineStr"/>
@@ -14877,7 +14877,7 @@
       <c r="B195" s="2" t="inlineStr"/>
       <c r="C195" s="2" t="inlineStr">
         <is>
-          <t>A0001035</t>
+          <t>TA-CONAVA</t>
         </is>
       </c>
       <c r="D195" s="2" t="inlineStr"/>
@@ -14951,7 +14951,7 @@
       <c r="B196" s="2" t="inlineStr"/>
       <c r="C196" s="2" t="inlineStr">
         <is>
-          <t>A0000651</t>
+          <t>TA-SELOIN</t>
         </is>
       </c>
       <c r="D196" s="2" t="inlineStr"/>
@@ -15025,7 +15025,7 @@
       <c r="B197" s="2" t="inlineStr"/>
       <c r="C197" s="2" t="inlineStr">
         <is>
-          <t>A0000652</t>
+          <t>TA-KEBATR</t>
         </is>
       </c>
       <c r="D197" s="2" t="inlineStr"/>
@@ -15099,7 +15099,7 @@
       <c r="B198" s="2" t="inlineStr"/>
       <c r="C198" s="2" t="inlineStr">
         <is>
-          <t>A0000653</t>
+          <t>TA-CODUBO</t>
         </is>
       </c>
       <c r="D198" s="2" t="inlineStr"/>
@@ -15173,7 +15173,7 @@
       <c r="B199" s="2" t="inlineStr"/>
       <c r="C199" s="2" t="inlineStr">
         <is>
-          <t>A0000656</t>
+          <t>TA-HODUDU</t>
         </is>
       </c>
       <c r="D199" s="2" t="inlineStr"/>
@@ -15247,7 +15247,7 @@
       <c r="B200" s="2" t="inlineStr"/>
       <c r="C200" s="2" t="inlineStr">
         <is>
-          <t>A0000660</t>
+          <t>DES-TUDANH</t>
         </is>
       </c>
       <c r="D200" s="2" t="inlineStr"/>
@@ -15321,7 +15321,7 @@
       <c r="B201" s="2" t="inlineStr"/>
       <c r="C201" s="2" t="inlineStr">
         <is>
-          <t>A0000661</t>
+          <t>DES-TUDANH-1</t>
         </is>
       </c>
       <c r="D201" s="2" t="inlineStr"/>
@@ -15395,7 +15395,7 @@
       <c r="B202" s="2" t="inlineStr"/>
       <c r="C202" s="2" t="inlineStr">
         <is>
-          <t>A0000662</t>
+          <t>TA-BIMA50</t>
         </is>
       </c>
       <c r="D202" s="2" t="inlineStr"/>
@@ -15469,7 +15469,7 @@
       <c r="B203" s="2" t="inlineStr"/>
       <c r="C203" s="2" t="inlineStr">
         <is>
-          <t>A0000663</t>
+          <t>TA-TICHBA</t>
         </is>
       </c>
       <c r="D203" s="2" t="inlineStr"/>
@@ -15543,7 +15543,7 @@
       <c r="B204" s="2" t="inlineStr"/>
       <c r="C204" s="2" t="inlineStr">
         <is>
-          <t>A0000664</t>
+          <t>TA-QUBAMA</t>
         </is>
       </c>
       <c r="D204" s="2" t="inlineStr"/>
@@ -15617,7 +15617,7 @@
       <c r="B205" s="2" t="inlineStr"/>
       <c r="C205" s="2" t="inlineStr">
         <is>
-          <t>A0000665</t>
+          <t>TA-QUBAMA-1</t>
         </is>
       </c>
       <c r="D205" s="2" t="inlineStr"/>
@@ -15691,7 +15691,7 @@
       <c r="B206" s="2" t="inlineStr"/>
       <c r="C206" s="2" t="inlineStr">
         <is>
-          <t>A0000666</t>
+          <t>TA-QUBAMA-2</t>
         </is>
       </c>
       <c r="D206" s="2" t="inlineStr"/>
@@ -15765,7 +15765,7 @@
       <c r="B207" s="2" t="inlineStr"/>
       <c r="C207" s="2" t="inlineStr">
         <is>
-          <t>A0000667</t>
+          <t>TA-QUBAMA-3</t>
         </is>
       </c>
       <c r="D207" s="2" t="inlineStr"/>
@@ -15839,7 +15839,7 @@
       <c r="B208" s="2" t="inlineStr"/>
       <c r="C208" s="2" t="inlineStr">
         <is>
-          <t>A0000670</t>
+          <t>DUA-DUNHPR-1</t>
         </is>
       </c>
       <c r="D208" s="2" t="inlineStr"/>
@@ -15913,7 +15913,7 @@
       <c r="B209" s="2" t="inlineStr"/>
       <c r="C209" s="2" t="inlineStr">
         <is>
-          <t>A0000673</t>
+          <t>DD-DEVOBA</t>
         </is>
       </c>
       <c r="D209" s="2" t="inlineStr"/>
@@ -15987,7 +15987,7 @@
       <c r="B210" s="2" t="inlineStr"/>
       <c r="C210" s="2" t="inlineStr">
         <is>
-          <t>A0000674</t>
+          <t>PED-THTUY</t>
         </is>
       </c>
       <c r="D210" s="2" t="inlineStr"/>
@@ -16061,7 +16061,7 @@
       <c r="B211" s="2" t="inlineStr"/>
       <c r="C211" s="2" t="inlineStr">
         <is>
-          <t>A0000675</t>
+          <t>PED-THMIBU</t>
         </is>
       </c>
       <c r="D211" s="2" t="inlineStr"/>
@@ -16135,7 +16135,7 @@
       <c r="B212" s="2" t="inlineStr"/>
       <c r="C212" s="2" t="inlineStr">
         <is>
-          <t>A0000676</t>
+          <t>PED-THDUMI</t>
         </is>
       </c>
       <c r="D212" s="2" t="inlineStr"/>
@@ -16209,7 +16209,7 @@
       <c r="B213" s="2" t="inlineStr"/>
       <c r="C213" s="2" t="inlineStr">
         <is>
-          <t>A0000680</t>
+          <t>DB-5XTI-1</t>
         </is>
       </c>
       <c r="D213" s="2" t="inlineStr"/>
@@ -16283,7 +16283,7 @@
       <c r="B214" s="2" t="inlineStr"/>
       <c r="C214" s="2" t="inlineStr">
         <is>
-          <t>A0000689</t>
+          <t>DB-4XTR</t>
         </is>
       </c>
       <c r="D214" s="2" t="inlineStr"/>
@@ -16357,7 +16357,7 @@
       <c r="B215" s="2" t="inlineStr"/>
       <c r="C215" s="2" t="inlineStr">
         <is>
-          <t>A0000690</t>
+          <t>BUT-BUQUTA-2</t>
         </is>
       </c>
       <c r="D215" s="2" t="inlineStr"/>
@@ -16431,7 +16431,7 @@
       <c r="B216" s="2" t="inlineStr"/>
       <c r="C216" s="2" t="inlineStr">
         <is>
-          <t>A0000693</t>
+          <t>DD-TABAKO</t>
         </is>
       </c>
       <c r="D216" s="2" t="inlineStr"/>
@@ -16505,7 +16505,7 @@
       <c r="B217" s="2" t="inlineStr"/>
       <c r="C217" s="2" t="inlineStr">
         <is>
-          <t>A0000694</t>
+          <t>DD-CHTHJA</t>
         </is>
       </c>
       <c r="D217" s="2" t="inlineStr"/>
@@ -16579,7 +16579,7 @@
       <c r="B218" s="2" t="inlineStr"/>
       <c r="C218" s="2" t="inlineStr">
         <is>
-          <t>A0000695</t>
+          <t>DB-MADAKH</t>
         </is>
       </c>
       <c r="D218" s="2" t="inlineStr"/>
@@ -16653,7 +16653,7 @@
       <c r="B219" s="2" t="inlineStr"/>
       <c r="C219" s="2" t="inlineStr">
         <is>
-          <t>A0000696</t>
+          <t>DB-BAMI3I</t>
         </is>
       </c>
       <c r="D219" s="2" t="inlineStr"/>
@@ -16727,7 +16727,7 @@
       <c r="B220" s="2" t="inlineStr"/>
       <c r="C220" s="2" t="inlineStr">
         <is>
-          <t>A0001079</t>
+          <t>DD-DECAVO</t>
         </is>
       </c>
       <c r="D220" s="2" t="inlineStr"/>
@@ -16801,7 +16801,7 @@
       <c r="B221" s="2" t="inlineStr"/>
       <c r="C221" s="2" t="inlineStr">
         <is>
-          <t>A0000699</t>
+          <t>DES-CHNGTR-1</t>
         </is>
       </c>
       <c r="D221" s="2" t="inlineStr"/>
@@ -16875,7 +16875,7 @@
       <c r="B222" s="2" t="inlineStr"/>
       <c r="C222" s="2" t="inlineStr">
         <is>
-          <t>A0000700</t>
+          <t>TA-CHGOCH</t>
         </is>
       </c>
       <c r="D222" s="2" t="inlineStr"/>
@@ -16949,7 +16949,7 @@
       <c r="B223" s="2" t="inlineStr"/>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>A0000704</t>
+          <t>TA-XOKECH</t>
         </is>
       </c>
       <c r="D223" s="2" t="inlineStr"/>
@@ -17023,7 +17023,7 @@
       <c r="B224" s="2" t="inlineStr"/>
       <c r="C224" s="2" t="inlineStr">
         <is>
-          <t>A0000706</t>
+          <t>TA-KETADA</t>
         </is>
       </c>
       <c r="D224" s="2" t="inlineStr"/>
@@ -17097,7 +17097,7 @@
       <c r="B225" s="2" t="inlineStr"/>
       <c r="C225" s="2" t="inlineStr">
         <is>
-          <t>A0000708</t>
+          <t>DB-BAGAKH</t>
         </is>
       </c>
       <c r="D225" s="2" t="inlineStr"/>
@@ -17171,7 +17171,7 @@
       <c r="B226" s="2" t="inlineStr"/>
       <c r="C226" s="2" t="inlineStr">
         <is>
-          <t>A0000709</t>
+          <t>DB-BAGAMO</t>
         </is>
       </c>
       <c r="D226" s="2" t="inlineStr"/>
@@ -17245,7 +17245,7 @@
       <c r="B227" s="2" t="inlineStr"/>
       <c r="C227" s="2" t="inlineStr">
         <is>
-          <t>A0000710</t>
+          <t>DB-CHDABO</t>
         </is>
       </c>
       <c r="D227" s="2" t="inlineStr"/>
@@ -17319,7 +17319,7 @@
       <c r="B228" s="2" t="inlineStr"/>
       <c r="C228" s="2" t="inlineStr">
         <is>
-          <t>A0000711</t>
+          <t>DB-BAGARA</t>
         </is>
       </c>
       <c r="D228" s="2" t="inlineStr"/>
@@ -17393,7 +17393,7 @@
       <c r="B229" s="2" t="inlineStr"/>
       <c r="C229" s="2" t="inlineStr">
         <is>
-          <t>A0000712</t>
+          <t>DB-5XDA</t>
         </is>
       </c>
       <c r="D229" s="2" t="inlineStr"/>
@@ -17467,7 +17467,7 @@
       <c r="B230" s="2" t="inlineStr"/>
       <c r="C230" s="2" t="inlineStr">
         <is>
-          <t>A0000713</t>
+          <t>DB-MTO</t>
         </is>
       </c>
       <c r="D230" s="2" t="inlineStr"/>
@@ -17541,7 +17541,7 @@
       <c r="B231" s="2" t="inlineStr"/>
       <c r="C231" s="2" t="inlineStr">
         <is>
-          <t>A0000714</t>
+          <t>DB-MNH-1</t>
         </is>
       </c>
       <c r="D231" s="2" t="inlineStr"/>
@@ -17615,7 +17615,7 @@
       <c r="B232" s="2" t="inlineStr"/>
       <c r="C232" s="2" t="inlineStr">
         <is>
-          <t>A0000715</t>
+          <t>DB-BAMI3I-1</t>
         </is>
       </c>
       <c r="D232" s="2" t="inlineStr"/>
@@ -17689,7 +17689,7 @@
       <c r="B233" s="2" t="inlineStr"/>
       <c r="C233" s="2" t="inlineStr">
         <is>
-          <t>A0000716</t>
+          <t>DB-2XDAVA</t>
         </is>
       </c>
       <c r="D233" s="2" t="inlineStr"/>
@@ -17763,7 +17763,7 @@
       <c r="B234" s="2" t="inlineStr"/>
       <c r="C234" s="2" t="inlineStr">
         <is>
-          <t>A0000717</t>
+          <t>BOT-BOMA56</t>
         </is>
       </c>
       <c r="D234" s="2" t="inlineStr"/>
@@ -17837,7 +17837,7 @@
       <c r="B235" s="2" t="inlineStr"/>
       <c r="C235" s="2" t="inlineStr">
         <is>
-          <t>A0000718</t>
+          <t>BOT-BOVI</t>
         </is>
       </c>
       <c r="D235" s="2" t="inlineStr"/>
@@ -17911,7 +17911,7 @@
       <c r="B236" s="2" t="inlineStr"/>
       <c r="C236" s="2" t="inlineStr">
         <is>
-          <t>A0001222</t>
+          <t>PED-MUNGCH</t>
         </is>
       </c>
       <c r="D236" s="2" t="inlineStr"/>
@@ -17985,7 +17985,7 @@
       <c r="B237" s="2" t="inlineStr"/>
       <c r="C237" s="2" t="inlineStr">
         <is>
-          <t>A0001009</t>
+          <t>PED-SUSC</t>
         </is>
       </c>
       <c r="D237" s="2" t="inlineStr"/>
@@ -18059,7 +18059,7 @@
       <c r="B238" s="2" t="inlineStr"/>
       <c r="C238" s="2" t="inlineStr">
         <is>
-          <t>A0000723</t>
+          <t>HC-KEMAVE</t>
         </is>
       </c>
       <c r="D238" s="2" t="inlineStr"/>
@@ -18133,7 +18133,7 @@
       <c r="B239" s="2" t="inlineStr"/>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>A0001231</t>
+          <t>HC-SOENSU</t>
         </is>
       </c>
       <c r="D239" s="2" t="inlineStr"/>
@@ -18207,7 +18207,7 @@
       <c r="B240" s="2" t="inlineStr"/>
       <c r="C240" s="2" t="inlineStr">
         <is>
-          <t>A0001230</t>
+          <t>HC-SOENSU-1</t>
         </is>
       </c>
       <c r="D240" s="2" t="inlineStr"/>
@@ -18281,7 +18281,7 @@
       <c r="B241" s="2" t="inlineStr"/>
       <c r="C241" s="2" t="inlineStr">
         <is>
-          <t>A0000730</t>
+          <t>DD-MAUL2L</t>
         </is>
       </c>
       <c r="D241" s="2" t="inlineStr"/>
@@ -18355,7 +18355,7 @@
       <c r="B242" s="2" t="inlineStr"/>
       <c r="C242" s="2" t="inlineStr">
         <is>
-          <t>A0000731</t>
+          <t>DES-NHDUA</t>
         </is>
       </c>
       <c r="D242" s="2" t="inlineStr"/>
@@ -18429,7 +18429,7 @@
       <c r="B243" s="2" t="inlineStr"/>
       <c r="C243" s="2" t="inlineStr">
         <is>
-          <t>A0000732</t>
+          <t>DES-NHDUB</t>
         </is>
       </c>
       <c r="D243" s="2" t="inlineStr"/>
@@ -18503,7 +18503,7 @@
       <c r="B244" s="2" t="inlineStr"/>
       <c r="C244" s="2" t="inlineStr">
         <is>
-          <t>A0000733</t>
+          <t>DES-NHDUC</t>
         </is>
       </c>
       <c r="D244" s="2" t="inlineStr"/>
@@ -18577,7 +18577,7 @@
       <c r="B245" s="2" t="inlineStr"/>
       <c r="C245" s="2" t="inlineStr">
         <is>
-          <t>A0000734</t>
+          <t>DES-NHBAPH</t>
         </is>
       </c>
       <c r="D245" s="2" t="inlineStr"/>
@@ -18651,7 +18651,7 @@
       <c r="B246" s="2" t="inlineStr"/>
       <c r="C246" s="2" t="inlineStr">
         <is>
-          <t>A0000735</t>
+          <t>TA-BANHNG</t>
         </is>
       </c>
       <c r="D246" s="2" t="inlineStr"/>
@@ -18725,7 +18725,7 @@
       <c r="B247" s="2" t="inlineStr"/>
       <c r="C247" s="2" t="inlineStr">
         <is>
-          <t>A0000736</t>
+          <t>DES-BAFO3G</t>
         </is>
       </c>
       <c r="D247" s="2" t="inlineStr"/>
@@ -18799,7 +18799,7 @@
       <c r="B248" s="2" t="inlineStr"/>
       <c r="C248" s="2" t="inlineStr">
         <is>
-          <t>A0000737</t>
+          <t>TA-TILAMA-1</t>
         </is>
       </c>
       <c r="D248" s="2" t="inlineStr"/>
@@ -18873,7 +18873,7 @@
       <c r="B249" s="2" t="inlineStr"/>
       <c r="C249" s="2" t="inlineStr">
         <is>
-          <t>A0000738</t>
+          <t>TA-NACHMA-1</t>
         </is>
       </c>
       <c r="D249" s="2" t="inlineStr"/>
@@ -18947,7 +18947,7 @@
       <c r="B250" s="2" t="inlineStr"/>
       <c r="C250" s="2" t="inlineStr">
         <is>
-          <t>A0000739</t>
+          <t>TA-CHVESI</t>
         </is>
       </c>
       <c r="D250" s="2" t="inlineStr"/>
@@ -19021,7 +19021,7 @@
       <c r="B251" s="2" t="inlineStr"/>
       <c r="C251" s="2" t="inlineStr">
         <is>
-          <t>A0000743</t>
+          <t>TA-CHSOKH</t>
         </is>
       </c>
       <c r="D251" s="2" t="inlineStr"/>
@@ -19095,7 +19095,7 @@
       <c r="B252" s="2" t="inlineStr"/>
       <c r="C252" s="2" t="inlineStr">
         <is>
-          <t>A0001164</t>
+          <t>TA-CHPRKH</t>
         </is>
       </c>
       <c r="D252" s="2" t="inlineStr"/>
@@ -19169,7 +19169,7 @@
       <c r="B253" s="2" t="inlineStr"/>
       <c r="C253" s="2" t="inlineStr">
         <is>
-          <t>A0001163</t>
+          <t>TA-CHBOKH</t>
         </is>
       </c>
       <c r="D253" s="2" t="inlineStr"/>
@@ -19243,7 +19243,7 @@
       <c r="B254" s="2" t="inlineStr"/>
       <c r="C254" s="2" t="inlineStr">
         <is>
-          <t>A0000746</t>
+          <t>TA-HODUPH</t>
         </is>
       </c>
       <c r="D254" s="2" t="inlineStr"/>
@@ -19317,7 +19317,7 @@
       <c r="B255" s="2" t="inlineStr"/>
       <c r="C255" s="2" t="inlineStr">
         <is>
-          <t>A0000752</t>
+          <t>BUT-BUCAGO-1</t>
         </is>
       </c>
       <c r="D255" s="2" t="inlineStr"/>
@@ -19391,7 +19391,7 @@
       <c r="B256" s="2" t="inlineStr"/>
       <c r="C256" s="2" t="inlineStr">
         <is>
-          <t>A0000753</t>
+          <t>BUT-BUDABO-2</t>
         </is>
       </c>
       <c r="D256" s="2" t="inlineStr"/>
@@ -19465,7 +19465,7 @@
       <c r="B257" s="2" t="inlineStr"/>
       <c r="C257" s="2" t="inlineStr">
         <is>
-          <t>A0000754</t>
+          <t>DD-TABATR-1</t>
         </is>
       </c>
       <c r="D257" s="2" t="inlineStr"/>
@@ -19539,7 +19539,7 @@
       <c r="B258" s="2" t="inlineStr"/>
       <c r="C258" s="2" t="inlineStr">
         <is>
-          <t>A0001056</t>
+          <t>TA-VOBITO</t>
         </is>
       </c>
       <c r="D258" s="2" t="inlineStr"/>
@@ -19613,7 +19613,7 @@
       <c r="B259" s="2" t="inlineStr"/>
       <c r="C259" s="2" t="inlineStr">
         <is>
-          <t>A0001057</t>
+          <t>TA-VOBINH</t>
         </is>
       </c>
       <c r="D259" s="2" t="inlineStr"/>
@@ -19687,7 +19687,7 @@
       <c r="B260" s="2" t="inlineStr"/>
       <c r="C260" s="2" t="inlineStr">
         <is>
-          <t>A0001185</t>
+          <t>GD-1KGE</t>
         </is>
       </c>
       <c r="D260" s="2" t="inlineStr"/>
@@ -19761,7 +19761,7 @@
       <c r="B261" s="2" t="inlineStr"/>
       <c r="C261" s="2" t="inlineStr">
         <is>
-          <t>A0001186</t>
+          <t>GD-1KGE-1</t>
         </is>
       </c>
       <c r="D261" s="2" t="inlineStr"/>
@@ -19835,7 +19835,7 @@
       <c r="B262" s="2" t="inlineStr"/>
       <c r="C262" s="2" t="inlineStr">
         <is>
-          <t>A0001189</t>
+          <t>GD-1KGE-2</t>
         </is>
       </c>
       <c r="D262" s="2" t="inlineStr"/>
@@ -19909,7 +19909,7 @@
       <c r="B263" s="2" t="inlineStr"/>
       <c r="C263" s="2" t="inlineStr">
         <is>
-          <t>A0001190</t>
+          <t>GD-1KGE-3</t>
         </is>
       </c>
       <c r="D263" s="2" t="inlineStr"/>
@@ -19983,7 +19983,7 @@
       <c r="B264" s="2" t="inlineStr"/>
       <c r="C264" s="2" t="inlineStr">
         <is>
-          <t>A0001191</t>
+          <t>GD-1KGE-4</t>
         </is>
       </c>
       <c r="D264" s="2" t="inlineStr"/>
@@ -20057,7 +20057,7 @@
       <c r="B265" s="2" t="inlineStr"/>
       <c r="C265" s="2" t="inlineStr">
         <is>
-          <t>A0000765</t>
+          <t>TA-CAFETH</t>
         </is>
       </c>
       <c r="D265" s="2" t="inlineStr"/>
@@ -20131,7 +20131,7 @@
       <c r="B266" s="2" t="inlineStr"/>
       <c r="C266" s="2" t="inlineStr">
         <is>
-          <t>A0000766</t>
+          <t>TA-CAFESA</t>
         </is>
       </c>
       <c r="D266" s="2" t="inlineStr"/>
@@ -20205,7 +20205,7 @@
       <c r="B267" s="2" t="inlineStr"/>
       <c r="C267" s="2" t="inlineStr">
         <is>
-          <t>A0000767</t>
+          <t>DB-XXSULT</t>
         </is>
       </c>
       <c r="D267" s="2" t="inlineStr"/>
@@ -20279,7 +20279,7 @@
       <c r="B268" s="2" t="inlineStr"/>
       <c r="C268" s="2" t="inlineStr">
         <is>
-          <t>A0000768</t>
+          <t>DB-XCTR</t>
         </is>
       </c>
       <c r="D268" s="2" t="inlineStr"/>
@@ -20353,7 +20353,7 @@
       <c r="B269" s="2" t="inlineStr"/>
       <c r="C269" s="2" t="inlineStr">
         <is>
-          <t>A0000769</t>
+          <t>DB-BAMISM</t>
         </is>
       </c>
       <c r="D269" s="2" t="inlineStr"/>
@@ -20427,7 +20427,7 @@
       <c r="B270" s="2" t="inlineStr"/>
       <c r="C270" s="2" t="inlineStr">
         <is>
-          <t>A0000771</t>
+          <t>DB-CBA</t>
         </is>
       </c>
       <c r="D270" s="2" t="inlineStr"/>
@@ -20501,7 +20501,7 @@
       <c r="B271" s="2" t="inlineStr"/>
       <c r="C271" s="2" t="inlineStr">
         <is>
-          <t>A0000772</t>
+          <t>DB-BAKHTR</t>
         </is>
       </c>
       <c r="D271" s="2" t="inlineStr"/>
@@ -20575,7 +20575,7 @@
       <c r="B272" s="2" t="inlineStr"/>
       <c r="C272" s="2" t="inlineStr">
         <is>
-          <t>A0000773</t>
+          <t>DB-XXHOCU</t>
         </is>
       </c>
       <c r="D272" s="2" t="inlineStr"/>
@@ -20649,7 +20649,7 @@
       <c r="B273" s="2" t="inlineStr"/>
       <c r="C273" s="2" t="inlineStr">
         <is>
-          <t>A0000781</t>
+          <t>HC-BACO15</t>
         </is>
       </c>
       <c r="D273" s="2" t="inlineStr"/>
@@ -20723,7 +20723,7 @@
       <c r="B274" s="2" t="inlineStr"/>
       <c r="C274" s="2" t="inlineStr">
         <is>
-          <t>A0000782</t>
+          <t>SM-SOMASO</t>
         </is>
       </c>
       <c r="D274" s="2" t="inlineStr"/>
@@ -20797,7 +20797,7 @@
       <c r="B275" s="2" t="inlineStr"/>
       <c r="C275" s="2" t="inlineStr">
         <is>
-          <t>A0000783</t>
+          <t>SM-SO14QU</t>
         </is>
       </c>
       <c r="D275" s="2" t="inlineStr"/>
@@ -20871,7 +20871,7 @@
       <c r="B276" s="2" t="inlineStr"/>
       <c r="C276" s="2" t="inlineStr">
         <is>
-          <t>A0000994</t>
+          <t>DD-MAHUBU</t>
         </is>
       </c>
       <c r="D276" s="2" t="inlineStr"/>
@@ -20945,7 +20945,7 @@
       <c r="B277" s="2" t="inlineStr"/>
       <c r="C277" s="2" t="inlineStr">
         <is>
-          <t>A0000786</t>
+          <t>DUA-DUBOHO</t>
         </is>
       </c>
       <c r="D277" s="2" t="inlineStr"/>
@@ -21019,7 +21019,7 @@
       <c r="B278" s="2" t="inlineStr"/>
       <c r="C278" s="2" t="inlineStr">
         <is>
-          <t>A0001216</t>
+          <t>TIP-TITHST</t>
         </is>
       </c>
       <c r="D278" s="2" t="inlineStr"/>
@@ -21093,7 +21093,7 @@
       <c r="B279" s="2" t="inlineStr"/>
       <c r="C279" s="2" t="inlineStr">
         <is>
-          <t>A0001218</t>
+          <t>TA-VONHTR-3</t>
         </is>
       </c>
       <c r="D279" s="2" t="inlineStr"/>
@@ -21167,7 +21167,7 @@
       <c r="B280" s="2" t="inlineStr"/>
       <c r="C280" s="2" t="inlineStr">
         <is>
-          <t>A0001219</t>
+          <t>TA-VONHTR-4</t>
         </is>
       </c>
       <c r="D280" s="2" t="inlineStr"/>
@@ -21241,7 +21241,7 @@
       <c r="B281" s="2" t="inlineStr"/>
       <c r="C281" s="2" t="inlineStr">
         <is>
-          <t>A0000790</t>
+          <t>TA-VONHTR-5</t>
         </is>
       </c>
       <c r="D281" s="2" t="inlineStr"/>
@@ -21315,7 +21315,7 @@
       <c r="B282" s="2" t="inlineStr"/>
       <c r="C282" s="2" t="inlineStr">
         <is>
-          <t>A0000791</t>
+          <t>DES-SEHODA</t>
         </is>
       </c>
       <c r="D282" s="2" t="inlineStr"/>
@@ -21389,7 +21389,7 @@
       <c r="B283" s="2" t="inlineStr"/>
       <c r="C283" s="2" t="inlineStr">
         <is>
-          <t>A0000792</t>
+          <t>DES-SEHODA-1</t>
         </is>
       </c>
       <c r="D283" s="2" t="inlineStr"/>
@@ -21463,7 +21463,7 @@
       <c r="B284" s="2" t="inlineStr"/>
       <c r="C284" s="2" t="inlineStr">
         <is>
-          <t>A0000793</t>
+          <t>DD-SEHODA</t>
         </is>
       </c>
       <c r="D284" s="2" t="inlineStr"/>
@@ -21537,7 +21537,7 @@
       <c r="B285" s="2" t="inlineStr"/>
       <c r="C285" s="2" t="inlineStr">
         <is>
-          <t>A0000794</t>
+          <t>DES-SEHODA-2</t>
         </is>
       </c>
       <c r="D285" s="2" t="inlineStr"/>
@@ -21611,7 +21611,7 @@
       <c r="B286" s="2" t="inlineStr"/>
       <c r="C286" s="2" t="inlineStr">
         <is>
-          <t>A0000795</t>
+          <t>HC-KEMAVE-1</t>
         </is>
       </c>
       <c r="D286" s="2" t="inlineStr"/>
@@ -21685,7 +21685,7 @@
       <c r="B287" s="2" t="inlineStr"/>
       <c r="C287" s="2" t="inlineStr">
         <is>
-          <t>A0001221</t>
+          <t>PED-CARE5K</t>
         </is>
       </c>
       <c r="D287" s="2" t="inlineStr"/>
@@ -21759,7 +21759,7 @@
       <c r="B288" s="2" t="inlineStr"/>
       <c r="C288" s="2" t="inlineStr">
         <is>
-          <t>A0001223</t>
+          <t>HC-XOMUNG</t>
         </is>
       </c>
       <c r="D288" s="2" t="inlineStr"/>
@@ -21833,7 +21833,7 @@
       <c r="B289" s="2" t="inlineStr"/>
       <c r="C289" s="2" t="inlineStr">
         <is>
-          <t>A0001046</t>
+          <t>TA-CHQUBA</t>
         </is>
       </c>
       <c r="D289" s="2" t="inlineStr"/>
@@ -21907,7 +21907,7 @@
       <c r="B290" s="2" t="inlineStr"/>
       <c r="C290" s="2" t="inlineStr">
         <is>
-          <t>A0000802</t>
+          <t>DB-4XDAVA</t>
         </is>
       </c>
       <c r="D290" s="2" t="inlineStr"/>
@@ -21981,7 +21981,7 @@
       <c r="B291" s="2" t="inlineStr"/>
       <c r="C291" s="2" t="inlineStr">
         <is>
-          <t>A0001026</t>
+          <t>TA-KINGD0</t>
         </is>
       </c>
       <c r="D291" s="2" t="inlineStr"/>
@@ -22055,7 +22055,7 @@
       <c r="B292" s="2" t="inlineStr"/>
       <c r="C292" s="2" t="inlineStr">
         <is>
-          <t>A0000805</t>
+          <t>TA-CADADA-1</t>
         </is>
       </c>
       <c r="D292" s="2" t="inlineStr"/>
@@ -22129,7 +22129,7 @@
       <c r="B293" s="2" t="inlineStr"/>
       <c r="C293" s="2" t="inlineStr">
         <is>
-          <t>A0000996</t>
+          <t>HC-ACE5L</t>
         </is>
       </c>
       <c r="D293" s="2" t="inlineStr"/>
@@ -22203,7 +22203,7 @@
       <c r="B294" s="2" t="inlineStr"/>
       <c r="C294" s="2" t="inlineStr">
         <is>
-          <t>A0000995</t>
+          <t>HC-COIP5L</t>
         </is>
       </c>
       <c r="D294" s="2" t="inlineStr"/>
@@ -22277,7 +22277,7 @@
       <c r="B295" s="2" t="inlineStr"/>
       <c r="C295" s="2" t="inlineStr">
         <is>
-          <t>A0000811</t>
+          <t>HC-ACE1L</t>
         </is>
       </c>
       <c r="D295" s="2" t="inlineStr"/>
@@ -22351,7 +22351,7 @@
       <c r="B296" s="2" t="inlineStr"/>
       <c r="C296" s="2" t="inlineStr">
         <is>
-          <t>A0000816</t>
+          <t>TA-TITH50</t>
         </is>
       </c>
       <c r="D296" s="2" t="inlineStr"/>
@@ -22425,7 +22425,7 @@
       <c r="B297" s="2" t="inlineStr"/>
       <c r="C297" s="2" t="inlineStr">
         <is>
-          <t>A0001091</t>
+          <t>DES-GEVETR</t>
         </is>
       </c>
       <c r="D297" s="2" t="inlineStr"/>
@@ -22499,7 +22499,7 @@
       <c r="B298" s="2" t="inlineStr"/>
       <c r="C298" s="2" t="inlineStr">
         <is>
-          <t>A0001069</t>
+          <t>SM-SOMAMI</t>
         </is>
       </c>
       <c r="D298" s="2" t="inlineStr"/>
@@ -22573,7 +22573,7 @@
       <c r="B299" s="2" t="inlineStr"/>
       <c r="C299" s="2" t="inlineStr">
         <is>
-          <t>A0000821</t>
+          <t>SM-FLDICA</t>
         </is>
       </c>
       <c r="D299" s="2" t="inlineStr"/>
@@ -22647,7 +22647,7 @@
       <c r="B300" s="2" t="inlineStr"/>
       <c r="C300" s="2" t="inlineStr">
         <is>
-          <t>A0000822</t>
+          <t>DES-SEPHNE</t>
         </is>
       </c>
       <c r="D300" s="2" t="inlineStr"/>
@@ -22721,7 +22721,7 @@
       <c r="B301" s="2" t="inlineStr"/>
       <c r="C301" s="2" t="inlineStr">
         <is>
-          <t>A0001188</t>
+          <t>GD-1KGE-5</t>
         </is>
       </c>
       <c r="D301" s="2" t="inlineStr"/>
@@ -22795,7 +22795,7 @@
       <c r="B302" s="2" t="inlineStr"/>
       <c r="C302" s="2" t="inlineStr">
         <is>
-          <t>A0001187</t>
+          <t>GD-1KGE-6</t>
         </is>
       </c>
       <c r="D302" s="2" t="inlineStr"/>
@@ -22869,7 +22869,7 @@
       <c r="B303" s="2" t="inlineStr"/>
       <c r="C303" s="2" t="inlineStr">
         <is>
-          <t>A0000830</t>
+          <t>DB-MTO-1</t>
         </is>
       </c>
       <c r="D303" s="2" t="inlineStr"/>
@@ -22943,7 +22943,7 @@
       <c r="B304" s="2" t="inlineStr"/>
       <c r="C304" s="2" t="inlineStr">
         <is>
-          <t>A0000831</t>
+          <t>DB-BAGA20</t>
         </is>
       </c>
       <c r="D304" s="2" t="inlineStr"/>
@@ -23017,7 +23017,7 @@
       <c r="B305" s="2" t="inlineStr"/>
       <c r="C305" s="2" t="inlineStr">
         <is>
-          <t>A0000832</t>
+          <t>DB-PHASHE</t>
         </is>
       </c>
       <c r="D305" s="2" t="inlineStr"/>
@@ -23091,7 +23091,7 @@
       <c r="B306" s="2" t="inlineStr"/>
       <c r="C306" s="2" t="inlineStr">
         <is>
-          <t>A0000833</t>
+          <t>DB-MITHM</t>
         </is>
       </c>
       <c r="D306" s="2" t="inlineStr"/>
@@ -23165,7 +23165,7 @@
       <c r="B307" s="2" t="inlineStr"/>
       <c r="C307" s="2" t="inlineStr">
         <is>
-          <t>A0000834</t>
+          <t>TC-TOCOTI-2</t>
         </is>
       </c>
       <c r="D307" s="2" t="inlineStr"/>
@@ -23239,7 +23239,7 @@
       <c r="B308" s="2" t="inlineStr"/>
       <c r="C308" s="2" t="inlineStr">
         <is>
-          <t>A0000836</t>
+          <t>DES-LIGEVE</t>
         </is>
       </c>
       <c r="D308" s="2" t="inlineStr"/>
@@ -23313,7 +23313,7 @@
       <c r="B309" s="2" t="inlineStr"/>
       <c r="C309" s="2" t="inlineStr">
         <is>
-          <t>A0000841</t>
+          <t>DD-DEBATR</t>
         </is>
       </c>
       <c r="D309" s="2" t="inlineStr"/>
@@ -23387,7 +23387,7 @@
       <c r="B310" s="2" t="inlineStr"/>
       <c r="C310" s="2" t="inlineStr">
         <is>
-          <t>A0001018</t>
+          <t>DUA-DUMONH</t>
         </is>
       </c>
       <c r="D310" s="2" t="inlineStr"/>
@@ -23461,7 +23461,7 @@
       <c r="B311" s="2" t="inlineStr"/>
       <c r="C311" s="2" t="inlineStr">
         <is>
-          <t>A0000845</t>
+          <t>DUA-DUMONH-1</t>
         </is>
       </c>
       <c r="D311" s="2" t="inlineStr"/>
@@ -23535,7 +23535,7 @@
       <c r="B312" s="2" t="inlineStr"/>
       <c r="C312" s="2" t="inlineStr">
         <is>
-          <t>A0001131</t>
+          <t>BOT-BOCL</t>
         </is>
       </c>
       <c r="D312" s="2" t="inlineStr"/>
@@ -23609,7 +23609,7 @@
       <c r="B313" s="2" t="inlineStr"/>
       <c r="C313" s="2" t="inlineStr">
         <is>
-          <t>A0001125</t>
+          <t>BOT-BONA-1</t>
         </is>
       </c>
       <c r="D313" s="2" t="inlineStr"/>
@@ -23683,7 +23683,7 @@
       <c r="B314" s="2" t="inlineStr"/>
       <c r="C314" s="2" t="inlineStr">
         <is>
-          <t>A0001106</t>
+          <t>HC-CHBACO</t>
         </is>
       </c>
       <c r="D314" s="2" t="inlineStr"/>
@@ -23757,7 +23757,7 @@
       <c r="B315" s="2" t="inlineStr"/>
       <c r="C315" s="2" t="inlineStr">
         <is>
-          <t>A0001215</t>
+          <t>TA-GILACH</t>
         </is>
       </c>
       <c r="D315" s="2" t="inlineStr"/>
@@ -23831,7 +23831,7 @@
       <c r="B316" s="2" t="inlineStr"/>
       <c r="C316" s="2" t="inlineStr">
         <is>
-          <t>A0000863</t>
+          <t>TA-GATANI</t>
         </is>
       </c>
       <c r="D316" s="2" t="inlineStr"/>
@@ -23905,7 +23905,7 @@
       <c r="B317" s="2" t="inlineStr"/>
       <c r="C317" s="2" t="inlineStr">
         <is>
-          <t>A0000864</t>
+          <t>TA-GATANI-1</t>
         </is>
       </c>
       <c r="D317" s="2" t="inlineStr"/>
@@ -23979,7 +23979,7 @@
       <c r="B318" s="2" t="inlineStr"/>
       <c r="C318" s="2" t="inlineStr">
         <is>
-          <t>A0000866</t>
+          <t>TA-VONHTI-1</t>
         </is>
       </c>
       <c r="D318" s="2" t="inlineStr"/>
@@ -24053,7 +24053,7 @@
       <c r="B319" s="2" t="inlineStr"/>
       <c r="C319" s="2" t="inlineStr">
         <is>
-          <t>A0000869</t>
+          <t>TA-CODUBO-1</t>
         </is>
       </c>
       <c r="D319" s="2" t="inlineStr"/>
@@ -24127,7 +24127,7 @@
       <c r="B320" s="2" t="inlineStr"/>
       <c r="C320" s="2" t="inlineStr">
         <is>
-          <t>A0001078</t>
+          <t>TA-HODUTI</t>
         </is>
       </c>
       <c r="D320" s="2" t="inlineStr"/>
@@ -24201,7 +24201,7 @@
       <c r="B321" s="2" t="inlineStr"/>
       <c r="C321" s="2" t="inlineStr">
         <is>
-          <t>A0000874</t>
+          <t>TA-TILAMA-2</t>
         </is>
       </c>
       <c r="D321" s="2" t="inlineStr"/>
@@ -24275,7 +24275,7 @@
       <c r="B322" s="2" t="inlineStr"/>
       <c r="C322" s="2" t="inlineStr">
         <is>
-          <t>A0000875</t>
+          <t>TA-KETACA</t>
         </is>
       </c>
       <c r="D322" s="2" t="inlineStr"/>
@@ -24349,7 +24349,7 @@
       <c r="B323" s="2" t="inlineStr"/>
       <c r="C323" s="2" t="inlineStr">
         <is>
-          <t>A0000876</t>
+          <t>TA-KETACA-1</t>
         </is>
       </c>
       <c r="D323" s="2" t="inlineStr"/>
@@ -24423,7 +24423,7 @@
       <c r="B324" s="2" t="inlineStr"/>
       <c r="C324" s="2" t="inlineStr">
         <is>
-          <t>A0000877</t>
+          <t>TA-KETACA-2</t>
         </is>
       </c>
       <c r="D324" s="2" t="inlineStr"/>
@@ -24497,7 +24497,7 @@
       <c r="B325" s="2" t="inlineStr"/>
       <c r="C325" s="2" t="inlineStr">
         <is>
-          <t>A0001064</t>
+          <t>DD-MABADI</t>
         </is>
       </c>
       <c r="D325" s="2" t="inlineStr"/>
@@ -24571,7 +24571,7 @@
       <c r="B326" s="2" t="inlineStr"/>
       <c r="C326" s="2" t="inlineStr">
         <is>
-          <t>A0001033</t>
+          <t>DD-DEPICA</t>
         </is>
       </c>
       <c r="D326" s="2" t="inlineStr"/>
@@ -24645,7 +24645,7 @@
       <c r="B327" s="2" t="inlineStr"/>
       <c r="C327" s="2" t="inlineStr">
         <is>
-          <t>A0000880</t>
+          <t>DD-PITHDE</t>
         </is>
       </c>
       <c r="D327" s="2" t="inlineStr"/>
@@ -24719,7 +24719,7 @@
       <c r="B328" s="2" t="inlineStr"/>
       <c r="C328" s="2" t="inlineStr">
         <is>
-          <t>A0001123</t>
+          <t>HC-TIDATR</t>
         </is>
       </c>
       <c r="D328" s="2" t="inlineStr"/>
@@ -24793,7 +24793,7 @@
       <c r="B329" s="2" t="inlineStr"/>
       <c r="C329" s="2" t="inlineStr">
         <is>
-          <t>A0000885</t>
+          <t>HC-NUCAMA</t>
         </is>
       </c>
       <c r="D329" s="2" t="inlineStr"/>
@@ -24867,7 +24867,7 @@
       <c r="B330" s="2" t="inlineStr"/>
       <c r="C330" s="2" t="inlineStr">
         <is>
-          <t>A0001235</t>
+          <t>BOT-BONA-2</t>
         </is>
       </c>
       <c r="D330" s="2" t="inlineStr"/>
@@ -24941,7 +24941,7 @@
       <c r="B331" s="2" t="inlineStr"/>
       <c r="C331" s="2" t="inlineStr">
         <is>
-          <t>A0001133</t>
+          <t>BOT-BOCR</t>
         </is>
       </c>
       <c r="D331" s="2" t="inlineStr"/>
@@ -25015,7 +25015,7 @@
       <c r="B332" s="2" t="inlineStr"/>
       <c r="C332" s="2" t="inlineStr">
         <is>
-          <t>A0000997</t>
+          <t>HC-LIMAJ2</t>
         </is>
       </c>
       <c r="D332" s="2" t="inlineStr"/>
@@ -25089,7 +25089,7 @@
       <c r="B333" s="2" t="inlineStr"/>
       <c r="C333" s="2" t="inlineStr">
         <is>
-          <t>A0001121</t>
+          <t>HC-LIJ2C2</t>
         </is>
       </c>
       <c r="D333" s="2" t="inlineStr"/>
@@ -25163,7 +25163,7 @@
       <c r="B334" s="2" t="inlineStr"/>
       <c r="C334" s="2" t="inlineStr">
         <is>
-          <t>A0001120</t>
+          <t>HC-LIJ2C0</t>
         </is>
       </c>
       <c r="D334" s="2" t="inlineStr"/>
@@ -25237,7 +25237,7 @@
       <c r="B335" s="2" t="inlineStr"/>
       <c r="C335" s="2" t="inlineStr">
         <is>
-          <t>A0001237</t>
+          <t>BOT-BOSU</t>
         </is>
       </c>
       <c r="D335" s="2" t="inlineStr"/>
@@ -25311,7 +25311,7 @@
       <c r="B336" s="2" t="inlineStr"/>
       <c r="C336" s="2" t="inlineStr">
         <is>
-          <t>A0001240</t>
+          <t>BOT-BOOM</t>
         </is>
       </c>
       <c r="D336" s="2" t="inlineStr"/>
@@ -25385,7 +25385,7 @@
       <c r="B337" s="2" t="inlineStr"/>
       <c r="C337" s="2" t="inlineStr">
         <is>
-          <t>A0001236</t>
+          <t>BOT-BOMI</t>
         </is>
       </c>
       <c r="D337" s="2" t="inlineStr"/>
@@ -25459,7 +25459,7 @@
       <c r="B338" s="2" t="inlineStr"/>
       <c r="C338" s="2" t="inlineStr">
         <is>
-          <t>A0001233</t>
+          <t>BOT-BOMA</t>
         </is>
       </c>
       <c r="D338" s="2" t="inlineStr"/>
@@ -25533,7 +25533,7 @@
       <c r="B339" s="2" t="inlineStr"/>
       <c r="C339" s="2" t="inlineStr">
         <is>
-          <t>A0001132</t>
+          <t>BOT-BOMA-1</t>
         </is>
       </c>
       <c r="D339" s="2" t="inlineStr"/>
@@ -25607,7 +25607,7 @@
       <c r="B340" s="2" t="inlineStr"/>
       <c r="C340" s="2" t="inlineStr">
         <is>
-          <t>A0001234</t>
+          <t>BOT-BOMA-2</t>
         </is>
       </c>
       <c r="D340" s="2" t="inlineStr"/>
@@ -25681,7 +25681,7 @@
       <c r="B341" s="2" t="inlineStr"/>
       <c r="C341" s="2" t="inlineStr">
         <is>
-          <t>A0001239</t>
+          <t>BOT-BOCL-1</t>
         </is>
       </c>
       <c r="D341" s="2" t="inlineStr"/>
@@ -25755,7 +25755,7 @@
       <c r="B342" s="2" t="inlineStr"/>
       <c r="C342" s="2" t="inlineStr">
         <is>
-          <t>A0001136</t>
+          <t>HC-PRI500</t>
         </is>
       </c>
       <c r="D342" s="2" t="inlineStr"/>
@@ -25829,7 +25829,7 @@
       <c r="B343" s="2" t="inlineStr"/>
       <c r="C343" s="2" t="inlineStr">
         <is>
-          <t>A0000904</t>
+          <t>HC-BODR50</t>
         </is>
       </c>
       <c r="D343" s="2" t="inlineStr"/>
@@ -25903,7 +25903,7 @@
       <c r="B344" s="2" t="inlineStr"/>
       <c r="C344" s="2" t="inlineStr">
         <is>
-          <t>A0001036</t>
+          <t>DD-TABAMA</t>
         </is>
       </c>
       <c r="D344" s="2" t="inlineStr"/>
@@ -25977,7 +25977,7 @@
       <c r="B345" s="2" t="inlineStr"/>
       <c r="C345" s="2" t="inlineStr">
         <is>
-          <t>A0000906</t>
+          <t>TA-CAFETH-1</t>
         </is>
       </c>
       <c r="D345" s="2" t="inlineStr"/>
@@ -26051,7 +26051,7 @@
       <c r="B346" s="2" t="inlineStr"/>
       <c r="C346" s="2" t="inlineStr">
         <is>
-          <t>A0000907</t>
+          <t>TA-CAFESA-1</t>
         </is>
       </c>
       <c r="D346" s="2" t="inlineStr"/>
@@ -26125,7 +26125,7 @@
       <c r="B347" s="2" t="inlineStr"/>
       <c r="C347" s="2" t="inlineStr">
         <is>
-          <t>A0001067</t>
+          <t>TC-DITOCO</t>
         </is>
       </c>
       <c r="D347" s="2" t="inlineStr"/>
@@ -26199,7 +26199,7 @@
       <c r="B348" s="2" t="inlineStr"/>
       <c r="C348" s="2" t="inlineStr">
         <is>
-          <t>A0000909</t>
+          <t>TC-TOCOTI-3</t>
         </is>
       </c>
       <c r="D348" s="2" t="inlineStr"/>
@@ -26273,7 +26273,7 @@
       <c r="B349" s="2" t="inlineStr"/>
       <c r="C349" s="2" t="inlineStr">
         <is>
-          <t>A0000910</t>
+          <t>TC-1KTOCO</t>
         </is>
       </c>
       <c r="D349" s="2" t="inlineStr"/>
@@ -26347,7 +26347,7 @@
       <c r="B350" s="2" t="inlineStr"/>
       <c r="C350" s="2" t="inlineStr">
         <is>
-          <t>A0000911</t>
+          <t>TC-TOCOTI-4</t>
         </is>
       </c>
       <c r="D350" s="2" t="inlineStr"/>
@@ -26421,7 +26421,7 @@
       <c r="B351" s="2" t="inlineStr"/>
       <c r="C351" s="2" t="inlineStr">
         <is>
-          <t>A0000912</t>
+          <t>TA-CHCHXA</t>
         </is>
       </c>
       <c r="D351" s="2" t="inlineStr"/>
@@ -26495,7 +26495,7 @@
       <c r="B352" s="2" t="inlineStr"/>
       <c r="C352" s="2" t="inlineStr">
         <is>
-          <t>A0000913</t>
+          <t>TA-BUCA3</t>
         </is>
       </c>
       <c r="D352" s="2" t="inlineStr"/>
@@ -26569,7 +26569,7 @@
       <c r="B353" s="2" t="inlineStr"/>
       <c r="C353" s="2" t="inlineStr">
         <is>
-          <t>A0000914</t>
+          <t>PED-BUTR4</t>
         </is>
       </c>
       <c r="D353" s="2" t="inlineStr"/>
@@ -26643,7 +26643,7 @@
       <c r="B354" s="2" t="inlineStr"/>
       <c r="C354" s="2" t="inlineStr">
         <is>
-          <t>A0001065</t>
+          <t>DD-TABAMA-1</t>
         </is>
       </c>
       <c r="D354" s="2" t="inlineStr"/>
@@ -26717,7 +26717,7 @@
       <c r="B355" s="2" t="inlineStr"/>
       <c r="C355" s="2" t="inlineStr">
         <is>
-          <t>A0001058</t>
+          <t>DD-TABAMA-2</t>
         </is>
       </c>
       <c r="D355" s="2" t="inlineStr"/>
@@ -26791,7 +26791,7 @@
       <c r="B356" s="2" t="inlineStr"/>
       <c r="C356" s="2" t="inlineStr">
         <is>
-          <t>A0001045</t>
+          <t>DD-DELE96</t>
         </is>
       </c>
       <c r="D356" s="2" t="inlineStr"/>
@@ -26865,7 +26865,7 @@
       <c r="B357" s="2" t="inlineStr"/>
       <c r="C357" s="2" t="inlineStr">
         <is>
-          <t>A0000918</t>
+          <t>DD-DELE48</t>
         </is>
       </c>
       <c r="D357" s="2" t="inlineStr"/>
@@ -26939,7 +26939,7 @@
       <c r="B358" s="2" t="inlineStr"/>
       <c r="C358" s="2" t="inlineStr">
         <is>
-          <t>A0000919</t>
+          <t>PED-TILACH</t>
         </is>
       </c>
       <c r="D358" s="2" t="inlineStr"/>
@@ -27013,7 +27013,7 @@
       <c r="B359" s="2" t="inlineStr"/>
       <c r="C359" s="2" t="inlineStr">
         <is>
-          <t>A0000920</t>
+          <t>TA-CHSOTR</t>
         </is>
       </c>
       <c r="D359" s="2" t="inlineStr"/>
@@ -27087,7 +27087,7 @@
       <c r="B360" s="2" t="inlineStr"/>
       <c r="C360" s="2" t="inlineStr">
         <is>
-          <t>A0001161</t>
+          <t>TA-TUNILO</t>
         </is>
       </c>
       <c r="D360" s="2" t="inlineStr"/>
@@ -27161,7 +27161,7 @@
       <c r="B361" s="2" t="inlineStr"/>
       <c r="C361" s="2" t="inlineStr">
         <is>
-          <t>A0001055</t>
+          <t>TA-5IPEKI-1</t>
         </is>
       </c>
       <c r="D361" s="2" t="inlineStr"/>
@@ -27235,7 +27235,7 @@
       <c r="B362" s="2" t="inlineStr"/>
       <c r="C362" s="2" t="inlineStr">
         <is>
-          <t>A0000923</t>
+          <t>PED-THDUMI-1</t>
         </is>
       </c>
       <c r="D362" s="2" t="inlineStr"/>
@@ -27309,7 +27309,7 @@
       <c r="B363" s="2" t="inlineStr"/>
       <c r="C363" s="2" t="inlineStr">
         <is>
-          <t>A0000924</t>
+          <t>PED-THSLBU</t>
         </is>
       </c>
       <c r="D363" s="2" t="inlineStr"/>
@@ -27383,7 +27383,7 @@
       <c r="B364" s="2" t="inlineStr"/>
       <c r="C364" s="2" t="inlineStr">
         <is>
-          <t>A0000925</t>
+          <t>PED-THQUTA</t>
         </is>
       </c>
       <c r="D364" s="2" t="inlineStr"/>
@@ -27457,7 +27457,7 @@
       <c r="B365" s="2" t="inlineStr"/>
       <c r="C365" s="2" t="inlineStr">
         <is>
-          <t>A0000926</t>
+          <t>DD-DECAVO-1</t>
         </is>
       </c>
       <c r="D365" s="2" t="inlineStr"/>
@@ -27531,7 +27531,7 @@
       <c r="B366" s="2" t="inlineStr"/>
       <c r="C366" s="2" t="inlineStr">
         <is>
-          <t>A0000927</t>
+          <t>DD-DECAVO-2</t>
         </is>
       </c>
       <c r="D366" s="2" t="inlineStr"/>
@@ -27605,7 +27605,7 @@
       <c r="B367" s="2" t="inlineStr"/>
       <c r="C367" s="2" t="inlineStr">
         <is>
-          <t>A0000928</t>
+          <t>DB-4XTI-1</t>
         </is>
       </c>
       <c r="D367" s="2" t="inlineStr"/>
@@ -27679,7 +27679,7 @@
       <c r="B368" s="2" t="inlineStr"/>
       <c r="C368" s="2" t="inlineStr">
         <is>
-          <t>A0000929</t>
+          <t>DB-2XTIXA</t>
         </is>
       </c>
       <c r="D368" s="2" t="inlineStr"/>
@@ -27753,7 +27753,7 @@
       <c r="B369" s="2" t="inlineStr"/>
       <c r="C369" s="2" t="inlineStr">
         <is>
-          <t>A0001168</t>
+          <t>TA-LOKH50</t>
         </is>
       </c>
       <c r="D369" s="2" t="inlineStr"/>
@@ -27827,7 +27827,7 @@
       <c r="B370" s="2" t="inlineStr"/>
       <c r="C370" s="2" t="inlineStr">
         <is>
-          <t>A0001049</t>
+          <t>PED-CADACA</t>
         </is>
       </c>
       <c r="D370" s="2" t="inlineStr"/>
@@ -27901,7 +27901,7 @@
       <c r="B371" s="2" t="inlineStr"/>
       <c r="C371" s="2" t="inlineStr">
         <is>
-          <t>A0001176</t>
+          <t>PED-DALAMI</t>
         </is>
       </c>
       <c r="D371" s="2" t="inlineStr"/>
@@ -27975,7 +27975,7 @@
       <c r="B372" s="2" t="inlineStr"/>
       <c r="C372" s="2" t="inlineStr">
         <is>
-          <t>A0001159</t>
+          <t>DUA-DU80LU</t>
         </is>
       </c>
       <c r="D372" s="2" t="inlineStr"/>
@@ -28049,7 +28049,7 @@
       <c r="B373" s="2" t="inlineStr"/>
       <c r="C373" s="2" t="inlineStr">
         <is>
-          <t>A0001160</t>
+          <t>DUA-DU10LU</t>
         </is>
       </c>
       <c r="D373" s="2" t="inlineStr"/>
@@ -28123,7 +28123,7 @@
       <c r="B374" s="2" t="inlineStr"/>
       <c r="C374" s="2" t="inlineStr">
         <is>
-          <t>A0000935</t>
+          <t>DD-MASAKH</t>
         </is>
       </c>
       <c r="D374" s="2" t="inlineStr"/>
@@ -28197,7 +28197,7 @@
       <c r="B375" s="2" t="inlineStr"/>
       <c r="C375" s="2" t="inlineStr">
         <is>
-          <t>A0000936</t>
+          <t>TA-TIFA12</t>
         </is>
       </c>
       <c r="D375" s="2" t="inlineStr"/>
@@ -28271,7 +28271,7 @@
       <c r="B376" s="2" t="inlineStr"/>
       <c r="C376" s="2" t="inlineStr">
         <is>
-          <t>A0000937</t>
+          <t>TA-TIFA12-1</t>
         </is>
       </c>
       <c r="D376" s="2" t="inlineStr"/>
@@ -28345,7 +28345,7 @@
       <c r="B377" s="2" t="inlineStr"/>
       <c r="C377" s="2" t="inlineStr">
         <is>
-          <t>A0000938</t>
+          <t>TA-TIFA12-2</t>
         </is>
       </c>
       <c r="D377" s="2" t="inlineStr"/>
@@ -28419,7 +28419,7 @@
       <c r="B378" s="2" t="inlineStr"/>
       <c r="C378" s="2" t="inlineStr">
         <is>
-          <t>A0000939</t>
+          <t>TA-TIFA12-3</t>
         </is>
       </c>
       <c r="D378" s="2" t="inlineStr"/>
@@ -28493,7 +28493,7 @@
       <c r="B379" s="2" t="inlineStr"/>
       <c r="C379" s="2" t="inlineStr">
         <is>
-          <t>A0000940</t>
+          <t>HC-BACO50</t>
         </is>
       </c>
       <c r="D379" s="2" t="inlineStr"/>
@@ -28567,7 +28567,7 @@
       <c r="B380" s="2" t="inlineStr"/>
       <c r="C380" s="2" t="inlineStr">
         <is>
-          <t>A0001066</t>
+          <t>HC-LIGEVE</t>
         </is>
       </c>
       <c r="D380" s="2" t="inlineStr"/>
@@ -28641,7 +28641,7 @@
       <c r="B381" s="2" t="inlineStr"/>
       <c r="C381" s="2" t="inlineStr">
         <is>
-          <t>A0000942</t>
+          <t>HC-LIGEVE-1</t>
         </is>
       </c>
       <c r="D381" s="2" t="inlineStr"/>
@@ -28715,7 +28715,7 @@
       <c r="B382" s="2" t="inlineStr"/>
       <c r="C382" s="2" t="inlineStr">
         <is>
-          <t>A0000943</t>
+          <t>DB-4XHO</t>
         </is>
       </c>
       <c r="D382" s="2" t="inlineStr"/>
@@ -28789,7 +28789,7 @@
       <c r="B383" s="2" t="inlineStr"/>
       <c r="C383" s="2" t="inlineStr">
         <is>
-          <t>A0000944</t>
+          <t>DES-LIGEVE-1</t>
         </is>
       </c>
       <c r="D383" s="2" t="inlineStr"/>
@@ -28863,7 +28863,7 @@
       <c r="B384" s="2" t="inlineStr"/>
       <c r="C384" s="2" t="inlineStr">
         <is>
-          <t>A0000945</t>
+          <t>DES-LIGEVE-2</t>
         </is>
       </c>
       <c r="D384" s="2" t="inlineStr"/>
@@ -28937,7 +28937,7 @@
       <c r="B385" s="2" t="inlineStr"/>
       <c r="C385" s="2" t="inlineStr">
         <is>
-          <t>A0000947</t>
+          <t>TC-1KTOCO-1</t>
         </is>
       </c>
       <c r="D385" s="2" t="inlineStr"/>
@@ -29011,7 +29011,7 @@
       <c r="B386" s="2" t="inlineStr"/>
       <c r="C386" s="2" t="inlineStr">
         <is>
-          <t>A0000948</t>
+          <t>DB-4XC</t>
         </is>
       </c>
       <c r="D386" s="2" t="inlineStr"/>
@@ -29085,7 +29085,7 @@
       <c r="B387" s="2" t="inlineStr"/>
       <c r="C387" s="2" t="inlineStr">
         <is>
-          <t>A0000949</t>
+          <t>DB-TRNHSA</t>
         </is>
       </c>
       <c r="D387" s="2" t="inlineStr"/>
@@ -29159,7 +29159,7 @@
       <c r="B388" s="2" t="inlineStr"/>
       <c r="C388" s="2" t="inlineStr">
         <is>
-          <t>A0000950</t>
+          <t>DB-TRNHCH</t>
         </is>
       </c>
       <c r="D388" s="2" t="inlineStr"/>
@@ -29233,7 +29233,7 @@
       <c r="B389" s="2" t="inlineStr"/>
       <c r="C389" s="2" t="inlineStr">
         <is>
-          <t>A0001122</t>
+          <t>HC-LIJ2C7</t>
         </is>
       </c>
       <c r="D389" s="2" t="inlineStr"/>
@@ -29307,7 +29307,7 @@
       <c r="B390" s="2" t="inlineStr"/>
       <c r="C390" s="2" t="inlineStr">
         <is>
-          <t>A0001135</t>
+          <t>BOT-BOOM-1</t>
         </is>
       </c>
       <c r="D390" s="2" t="inlineStr"/>
@@ -29381,7 +29381,7 @@
       <c r="B391" s="2" t="inlineStr"/>
       <c r="C391" s="2" t="inlineStr">
         <is>
-          <t>A0000955</t>
+          <t>HC-LIEMJ2</t>
         </is>
       </c>
       <c r="D391" s="2" t="inlineStr"/>
@@ -29455,7 +29455,7 @@
       <c r="B392" s="2" t="inlineStr"/>
       <c r="C392" s="2" t="inlineStr">
         <is>
-          <t>A0000958</t>
+          <t>DB-4XDA-1</t>
         </is>
       </c>
       <c r="D392" s="2" t="inlineStr"/>
@@ -29529,7 +29529,7 @@
       <c r="B393" s="2" t="inlineStr"/>
       <c r="C393" s="2" t="inlineStr">
         <is>
-          <t>A0000960</t>
+          <t>DD-MOTAMA</t>
         </is>
       </c>
       <c r="D393" s="2" t="inlineStr"/>
@@ -29603,7 +29603,7 @@
       <c r="B394" s="2" t="inlineStr"/>
       <c r="C394" s="2" t="inlineStr">
         <is>
-          <t>A0000962</t>
+          <t>HC-SUWH25</t>
         </is>
       </c>
       <c r="D394" s="2" t="inlineStr"/>
@@ -29677,7 +29677,7 @@
       <c r="B395" s="2" t="inlineStr"/>
       <c r="C395" s="2" t="inlineStr">
         <is>
-          <t>A0000963</t>
+          <t>HC-SUBL25</t>
         </is>
       </c>
       <c r="D395" s="2" t="inlineStr"/>
@@ -29751,7 +29751,7 @@
       <c r="B396" s="2" t="inlineStr"/>
       <c r="C396" s="2" t="inlineStr">
         <is>
-          <t>A0000965</t>
+          <t>PED-SUSC-1</t>
         </is>
       </c>
       <c r="D396" s="2" t="inlineStr"/>
@@ -29825,7 +29825,7 @@
       <c r="B397" s="2" t="inlineStr"/>
       <c r="C397" s="2" t="inlineStr">
         <is>
-          <t>A0000966</t>
+          <t>HC-GESC</t>
         </is>
       </c>
       <c r="D397" s="2" t="inlineStr"/>
@@ -29899,7 +29899,7 @@
       <c r="B398" s="2" t="inlineStr"/>
       <c r="C398" s="2" t="inlineStr">
         <is>
-          <t>A0001155</t>
+          <t>TC-DITOCO-1</t>
         </is>
       </c>
       <c r="D398" s="2" t="inlineStr"/>
@@ -29973,7 +29973,7 @@
       <c r="B399" s="2" t="inlineStr"/>
       <c r="C399" s="2" t="inlineStr">
         <is>
-          <t>A0000974</t>
+          <t>TA-CODUBO-2</t>
         </is>
       </c>
       <c r="D399" s="2" t="inlineStr"/>
@@ -30047,7 +30047,7 @@
       <c r="B400" s="2" t="inlineStr"/>
       <c r="C400" s="2" t="inlineStr">
         <is>
-          <t>A0000975</t>
+          <t>TA-HUDUGE</t>
         </is>
       </c>
       <c r="D400" s="2" t="inlineStr"/>
@@ -30121,7 +30121,7 @@
       <c r="B401" s="2" t="inlineStr"/>
       <c r="C401" s="2" t="inlineStr">
         <is>
-          <t>A0000976</t>
+          <t>TA-HUDUGE-1</t>
         </is>
       </c>
       <c r="D401" s="2" t="inlineStr"/>
@@ -30195,7 +30195,7 @@
       <c r="B402" s="2" t="inlineStr"/>
       <c r="C402" s="2" t="inlineStr">
         <is>
-          <t>A0000979</t>
+          <t>TA-CHCHVA</t>
         </is>
       </c>
       <c r="D402" s="2" t="inlineStr"/>
@@ -30269,7 +30269,7 @@
       <c r="B403" s="2" t="inlineStr"/>
       <c r="C403" s="2" t="inlineStr">
         <is>
-          <t>A0000981</t>
+          <t>DD-DESAPI</t>
         </is>
       </c>
       <c r="D403" s="2" t="inlineStr"/>
@@ -30343,7 +30343,7 @@
       <c r="B404" s="2" t="inlineStr"/>
       <c r="C404" s="2" t="inlineStr">
         <is>
-          <t>DICH-VU</t>
+          <t>DV-SUCHTA</t>
         </is>
       </c>
       <c r="D404" s="2" t="inlineStr"/>
@@ -30413,7 +30413,7 @@
       <c r="B405" s="2" t="inlineStr"/>
       <c r="C405" s="2" t="inlineStr">
         <is>
-          <t>A0000951</t>
+          <t>DB-4XDATR-1</t>
         </is>
       </c>
       <c r="D405" s="2" t="inlineStr"/>
@@ -30487,7 +30487,7 @@
       <c r="B406" s="2" t="inlineStr"/>
       <c r="C406" s="2" t="inlineStr">
         <is>
-          <t>A0000952</t>
+          <t>DB-MVA</t>
         </is>
       </c>
       <c r="D406" s="2" t="inlineStr"/>
@@ -30561,7 +30561,7 @@
       <c r="B407" s="2" t="inlineStr"/>
       <c r="C407" s="2" t="inlineStr">
         <is>
-          <t>A0000956</t>
+          <t>DES-SEBONE</t>
         </is>
       </c>
       <c r="D407" s="2" t="inlineStr"/>
@@ -30635,7 +30635,7 @@
       <c r="B408" s="2" t="inlineStr"/>
       <c r="C408" s="2" t="inlineStr">
         <is>
-          <t>A0000957</t>
+          <t>DES-SEBUXO</t>
         </is>
       </c>
       <c r="D408" s="2" t="inlineStr"/>
@@ -30709,7 +30709,7 @@
       <c r="B409" s="2" t="inlineStr"/>
       <c r="C409" s="2" t="inlineStr">
         <is>
-          <t>A0000959</t>
+          <t>DD-THMATR</t>
         </is>
       </c>
       <c r="D409" s="2" t="inlineStr"/>
@@ -30783,7 +30783,7 @@
       <c r="B410" s="2" t="inlineStr"/>
       <c r="C410" s="2" t="inlineStr">
         <is>
-          <t>A0000961</t>
+          <t>DD-DACA3-1</t>
         </is>
       </c>
       <c r="D410" s="2" t="inlineStr"/>
@@ -30857,7 +30857,7 @@
       <c r="B411" s="2" t="inlineStr"/>
       <c r="C411" s="2" t="inlineStr">
         <is>
-          <t>A0000964</t>
+          <t>SM-SESOMA</t>
         </is>
       </c>
       <c r="D411" s="2" t="inlineStr"/>
@@ -30931,7 +30931,7 @@
       <c r="B412" s="2" t="inlineStr"/>
       <c r="C412" s="2" t="inlineStr">
         <is>
-          <t>A0000973</t>
+          <t>DES-GENA3D</t>
         </is>
       </c>
       <c r="D412" s="2" t="inlineStr"/>
@@ -31005,7 +31005,7 @@
       <c r="B413" s="2" t="inlineStr"/>
       <c r="C413" s="2" t="inlineStr">
         <is>
-          <t>A0000977</t>
+          <t>TA-KECHCA</t>
         </is>
       </c>
       <c r="D413" s="2" t="inlineStr"/>
@@ -31079,7 +31079,7 @@
       <c r="B414" s="2" t="inlineStr"/>
       <c r="C414" s="2" t="inlineStr">
         <is>
-          <t>A0000978</t>
+          <t>TA-KECHCA-1</t>
         </is>
       </c>
       <c r="D414" s="2" t="inlineStr"/>
@@ -31153,7 +31153,7 @@
       <c r="B415" s="2" t="inlineStr"/>
       <c r="C415" s="2" t="inlineStr">
         <is>
-          <t>A0000980</t>
+          <t>TA-CHQUBA-1</t>
         </is>
       </c>
       <c r="D415" s="2" t="inlineStr"/>
@@ -31227,7 +31227,7 @@
       <c r="B416" s="2" t="inlineStr"/>
       <c r="C416" s="2" t="inlineStr">
         <is>
-          <t>A0000983</t>
+          <t>PED-MUVIXO</t>
         </is>
       </c>
       <c r="D416" s="2" t="inlineStr"/>
@@ -31301,7 +31301,7 @@
       <c r="B417" s="2" t="inlineStr"/>
       <c r="C417" s="2" t="inlineStr">
         <is>
-          <t>A0000984</t>
+          <t>SM-MOCAEY</t>
         </is>
       </c>
       <c r="D417" s="2" t="inlineStr"/>
@@ -31375,7 +31375,7 @@
       <c r="B418" s="2" t="inlineStr"/>
       <c r="C418" s="2" t="inlineStr">
         <is>
-          <t>A0000985</t>
+          <t>HC-GETH30</t>
         </is>
       </c>
       <c r="D418" s="2" t="inlineStr"/>
@@ -31449,7 +31449,7 @@
       <c r="B419" s="2" t="inlineStr"/>
       <c r="C419" s="2" t="inlineStr">
         <is>
-          <t>A0000986</t>
+          <t>TC-DITOCO-2</t>
         </is>
       </c>
       <c r="D419" s="2" t="inlineStr"/>
@@ -31523,7 +31523,7 @@
       <c r="B420" s="2" t="inlineStr"/>
       <c r="C420" s="2" t="inlineStr">
         <is>
-          <t>A0000988</t>
+          <t>HC-GENA3D</t>
         </is>
       </c>
       <c r="D420" s="2" t="inlineStr"/>
@@ -31597,7 +31597,7 @@
       <c r="B421" s="2" t="inlineStr"/>
       <c r="C421" s="2" t="inlineStr">
         <is>
-          <t>A0001094</t>
+          <t>SM-SOMAMI-1</t>
         </is>
       </c>
       <c r="D421" s="2" t="inlineStr"/>
@@ -31671,7 +31671,7 @@
       <c r="B422" s="2" t="inlineStr"/>
       <c r="C422" s="2" t="inlineStr">
         <is>
-          <t>A0001003</t>
+          <t>HC-LIEMG3</t>
         </is>
       </c>
       <c r="D422" s="2" t="inlineStr"/>
@@ -31745,7 +31745,7 @@
       <c r="B423" s="2" t="inlineStr"/>
       <c r="C423" s="2" t="inlineStr">
         <is>
-          <t>A0001008</t>
+          <t>PED-XOGESC</t>
         </is>
       </c>
       <c r="D423" s="2" t="inlineStr"/>
@@ -31819,7 +31819,7 @@
       <c r="B424" s="2" t="inlineStr"/>
       <c r="C424" s="2" t="inlineStr">
         <is>
-          <t>A0001010</t>
+          <t>TA-VONHMY</t>
         </is>
       </c>
       <c r="D424" s="2" t="inlineStr"/>
@@ -31893,7 +31893,7 @@
       <c r="B425" s="2" t="inlineStr"/>
       <c r="C425" s="2" t="inlineStr">
         <is>
-          <t>A0001014</t>
+          <t>BUT-SE5CBU</t>
         </is>
       </c>
       <c r="D425" s="2" t="inlineStr"/>
@@ -31967,7 +31967,7 @@
       <c r="B426" s="2" t="inlineStr"/>
       <c r="C426" s="2" t="inlineStr">
         <is>
-          <t>A0001019</t>
+          <t>DUA-DUMO</t>
         </is>
       </c>
       <c r="D426" s="2" t="inlineStr"/>
@@ -32041,7 +32041,7 @@
       <c r="B427" s="2" t="inlineStr"/>
       <c r="C427" s="2" t="inlineStr">
         <is>
-          <t>A0001020</t>
+          <t>DUA-DUMO-1</t>
         </is>
       </c>
       <c r="D427" s="2" t="inlineStr"/>
@@ -32115,7 +32115,7 @@
       <c r="B428" s="2" t="inlineStr"/>
       <c r="C428" s="2" t="inlineStr">
         <is>
-          <t>A0001023</t>
+          <t>TIP-TITHNA</t>
         </is>
       </c>
       <c r="D428" s="2" t="inlineStr"/>
@@ -32189,7 +32189,7 @@
       <c r="B429" s="2" t="inlineStr"/>
       <c r="C429" s="2" t="inlineStr">
         <is>
-          <t>A0001024</t>
+          <t>PED-BINGKH</t>
         </is>
       </c>
       <c r="D429" s="2" t="inlineStr"/>
@@ -32263,7 +32263,7 @@
       <c r="B430" s="2" t="inlineStr"/>
       <c r="C430" s="2" t="inlineStr">
         <is>
-          <t>A0001025</t>
+          <t>BUT-BUCAGO-2</t>
         </is>
       </c>
       <c r="D430" s="2" t="inlineStr"/>
@@ -32337,7 +32337,7 @@
       <c r="B431" s="2" t="inlineStr"/>
       <c r="C431" s="2" t="inlineStr">
         <is>
-          <t>A0001029</t>
+          <t>DES-BLNH</t>
         </is>
       </c>
       <c r="D431" s="2" t="inlineStr"/>
@@ -32411,7 +32411,7 @@
       <c r="B432" s="2" t="inlineStr"/>
       <c r="C432" s="2" t="inlineStr">
         <is>
-          <t>A0001030</t>
+          <t>DES-BLNH-1</t>
         </is>
       </c>
       <c r="D432" s="2" t="inlineStr"/>
@@ -32485,7 +32485,7 @@
       <c r="B433" s="2" t="inlineStr"/>
       <c r="C433" s="2" t="inlineStr">
         <is>
-          <t>A0001037</t>
+          <t>HC-LIEMIT</t>
         </is>
       </c>
       <c r="D433" s="2" t="inlineStr"/>
@@ -32559,7 +32559,7 @@
       <c r="B434" s="2" t="inlineStr"/>
       <c r="C434" s="2" t="inlineStr">
         <is>
-          <t>B0000001</t>
+          <t>PED-BIDUMI</t>
         </is>
       </c>
       <c r="D434" s="2" t="inlineStr"/>
@@ -32633,7 +32633,7 @@
       <c r="B435" s="2" t="inlineStr"/>
       <c r="C435" s="2" t="inlineStr">
         <is>
-          <t>B0000002</t>
+          <t>PED-XOKECH</t>
         </is>
       </c>
       <c r="D435" s="2" t="inlineStr"/>
@@ -32707,7 +32707,7 @@
       <c r="B436" s="2" t="inlineStr"/>
       <c r="C436" s="2" t="inlineStr">
         <is>
-          <t>B0000003</t>
+          <t>PED-HOTUY</t>
         </is>
       </c>
       <c r="D436" s="2" t="inlineStr"/>
@@ -32781,7 +32781,7 @@
       <c r="B437" s="2" t="inlineStr"/>
       <c r="C437" s="2" t="inlineStr">
         <is>
-          <t>A0001044</t>
+          <t>PED-MUVI</t>
         </is>
       </c>
       <c r="D437" s="2" t="inlineStr"/>
@@ -32855,7 +32855,7 @@
       <c r="B438" s="2" t="inlineStr"/>
       <c r="C438" s="2" t="inlineStr">
         <is>
-          <t>A0001048</t>
+          <t>TA-CHBOCO</t>
         </is>
       </c>
       <c r="D438" s="2" t="inlineStr"/>
@@ -32929,7 +32929,7 @@
       <c r="B439" s="2" t="inlineStr"/>
       <c r="C439" s="2" t="inlineStr">
         <is>
-          <t>A0001051</t>
+          <t>PED-CADACA-1</t>
         </is>
       </c>
       <c r="D439" s="2" t="inlineStr"/>
@@ -33003,7 +33003,7 @@
       <c r="B440" s="2" t="inlineStr"/>
       <c r="C440" s="2" t="inlineStr">
         <is>
-          <t>A0001052</t>
+          <t>TA-KEACDU</t>
         </is>
       </c>
       <c r="D440" s="2" t="inlineStr"/>
@@ -33077,7 +33077,7 @@
       <c r="B441" s="2" t="inlineStr"/>
       <c r="C441" s="2" t="inlineStr">
         <is>
-          <t>B0000004</t>
+          <t>TA-BIQUTA</t>
         </is>
       </c>
       <c r="D441" s="2" t="inlineStr"/>
@@ -33151,7 +33151,7 @@
       <c r="B442" s="2" t="inlineStr"/>
       <c r="C442" s="2" t="inlineStr">
         <is>
-          <t>A0001059</t>
+          <t>DES-MAINSE</t>
         </is>
       </c>
       <c r="D442" s="2" t="inlineStr"/>
@@ -33225,7 +33225,7 @@
       <c r="B443" s="2" t="inlineStr"/>
       <c r="C443" s="2" t="inlineStr">
         <is>
-          <t>A0001060</t>
+          <t>TC-GEL6IN</t>
         </is>
       </c>
       <c r="D443" s="2" t="inlineStr"/>
@@ -33299,7 +33299,7 @@
       <c r="B444" s="2" t="inlineStr"/>
       <c r="C444" s="2" t="inlineStr">
         <is>
-          <t>A0001063</t>
+          <t>DD-MABADI-1</t>
         </is>
       </c>
       <c r="D444" s="2" t="inlineStr"/>
@@ -33373,7 +33373,7 @@
       <c r="B445" s="2" t="inlineStr"/>
       <c r="C445" s="2" t="inlineStr">
         <is>
-          <t>A0001068</t>
+          <t>HC-GEVEDE</t>
         </is>
       </c>
       <c r="D445" s="2" t="inlineStr"/>
@@ -33447,7 +33447,7 @@
       <c r="B446" s="2" t="inlineStr"/>
       <c r="C446" s="2" t="inlineStr">
         <is>
-          <t>A0001070</t>
+          <t>PED-5IPEKI</t>
         </is>
       </c>
       <c r="D446" s="2" t="inlineStr"/>
@@ -33521,7 +33521,7 @@
       <c r="B447" s="2" t="inlineStr"/>
       <c r="C447" s="2" t="inlineStr">
         <is>
-          <t>A0001071</t>
+          <t>PED-LEJE</t>
         </is>
       </c>
       <c r="D447" s="2" t="inlineStr"/>
@@ -33595,7 +33595,7 @@
       <c r="B448" s="2" t="inlineStr"/>
       <c r="C448" s="2" t="inlineStr">
         <is>
-          <t>A0001074</t>
+          <t>TA-KETACA-3</t>
         </is>
       </c>
       <c r="D448" s="2" t="inlineStr"/>
@@ -33669,7 +33669,7 @@
       <c r="B449" s="2" t="inlineStr"/>
       <c r="C449" s="2" t="inlineStr">
         <is>
-          <t>A0001075</t>
+          <t>TA-KETACA-4</t>
         </is>
       </c>
       <c r="D449" s="2" t="inlineStr"/>
@@ -33743,7 +33743,7 @@
       <c r="B450" s="2" t="inlineStr"/>
       <c r="C450" s="2" t="inlineStr">
         <is>
-          <t>A0001076</t>
+          <t>DD-DELELA</t>
         </is>
       </c>
       <c r="D450" s="2" t="inlineStr"/>
@@ -33817,7 +33817,7 @@
       <c r="B451" s="2" t="inlineStr"/>
       <c r="C451" s="2" t="inlineStr">
         <is>
-          <t>A0001077</t>
+          <t>DD-MAKHTR</t>
         </is>
       </c>
       <c r="D451" s="2" t="inlineStr"/>
@@ -33891,7 +33891,7 @@
       <c r="B452" s="2" t="inlineStr"/>
       <c r="C452" s="2" t="inlineStr">
         <is>
-          <t>A0001080</t>
+          <t>DB-MITHXF-1</t>
         </is>
       </c>
       <c r="D452" s="2" t="inlineStr"/>
@@ -33965,7 +33965,7 @@
       <c r="B453" s="2" t="inlineStr"/>
       <c r="C453" s="2" t="inlineStr">
         <is>
-          <t>A0001081</t>
+          <t>TA-KIBAMO</t>
         </is>
       </c>
       <c r="D453" s="2" t="inlineStr"/>
@@ -34039,7 +34039,7 @@
       <c r="B454" s="2" t="inlineStr"/>
       <c r="C454" s="2" t="inlineStr">
         <is>
-          <t>A0001109</t>
+          <t>TC-IMTOCO</t>
         </is>
       </c>
       <c r="D454" s="2" t="inlineStr"/>
@@ -34113,7 +34113,7 @@
       <c r="B455" s="2" t="inlineStr"/>
       <c r="C455" s="2" t="inlineStr">
         <is>
-          <t>A0001083</t>
+          <t>TC-IMTOCO-1</t>
         </is>
       </c>
       <c r="D455" s="2" t="inlineStr"/>
@@ -34187,7 +34187,7 @@
       <c r="B456" s="2" t="inlineStr"/>
       <c r="C456" s="2" t="inlineStr">
         <is>
-          <t>A0001153</t>
+          <t>TC-IMTOCO-2</t>
         </is>
       </c>
       <c r="D456" s="2" t="inlineStr"/>
@@ -34261,7 +34261,7 @@
       <c r="B457" s="2" t="inlineStr"/>
       <c r="C457" s="2" t="inlineStr">
         <is>
-          <t>A0001154</t>
+          <t>TC-IMTOCO-3</t>
         </is>
       </c>
       <c r="D457" s="2" t="inlineStr"/>
@@ -34335,7 +34335,7 @@
       <c r="B458" s="2" t="inlineStr"/>
       <c r="C458" s="2" t="inlineStr">
         <is>
-          <t>A0001150</t>
+          <t>TC-IMTOCO-4</t>
         </is>
       </c>
       <c r="D458" s="2" t="inlineStr"/>
@@ -34409,7 +34409,7 @@
       <c r="B459" s="2" t="inlineStr"/>
       <c r="C459" s="2" t="inlineStr">
         <is>
-          <t>A0001151</t>
+          <t>TC-IMTOCO-5</t>
         </is>
       </c>
       <c r="D459" s="2" t="inlineStr"/>
@@ -34483,7 +34483,7 @@
       <c r="B460" s="2" t="inlineStr"/>
       <c r="C460" s="2" t="inlineStr">
         <is>
-          <t>A0001089</t>
+          <t>SM-GLGEPO</t>
         </is>
       </c>
       <c r="D460" s="2" t="inlineStr"/>
@@ -34557,7 +34557,7 @@
       <c r="B461" s="2" t="inlineStr"/>
       <c r="C461" s="2" t="inlineStr">
         <is>
-          <t>A0001090</t>
+          <t>GD-BIA15M</t>
         </is>
       </c>
       <c r="D461" s="2" t="inlineStr"/>
@@ -34631,7 +34631,7 @@
       <c r="B462" s="2" t="inlineStr"/>
       <c r="C462" s="2" t="inlineStr">
         <is>
-          <t>A0001116</t>
+          <t>HC-CUOINA</t>
         </is>
       </c>
       <c r="D462" s="2" t="inlineStr"/>
@@ -34705,7 +34705,7 @@
       <c r="B463" s="2" t="inlineStr"/>
       <c r="C463" s="2" t="inlineStr">
         <is>
-          <t>A0001117</t>
+          <t>HC-LIQPRO</t>
         </is>
       </c>
       <c r="D463" s="2" t="inlineStr"/>
@@ -34779,7 +34779,7 @@
       <c r="B464" s="2" t="inlineStr"/>
       <c r="C464" s="2" t="inlineStr">
         <is>
-          <t>A0001214</t>
+          <t>HC-LIQWIN</t>
         </is>
       </c>
       <c r="D464" s="2" t="inlineStr"/>
@@ -34853,7 +34853,7 @@
       <c r="B465" s="2" t="inlineStr"/>
       <c r="C465" s="2" t="inlineStr">
         <is>
-          <t>A0001137</t>
+          <t>TA-COLIMI</t>
         </is>
       </c>
       <c r="D465" s="2" t="inlineStr"/>
@@ -34927,7 +34927,7 @@
       <c r="B466" s="2" t="inlineStr"/>
       <c r="C466" s="2" t="inlineStr">
         <is>
-          <t>A0001138</t>
+          <t>PED-DELACH</t>
         </is>
       </c>
       <c r="D466" s="2" t="inlineStr"/>
@@ -35001,7 +35001,7 @@
       <c r="B467" s="2" t="inlineStr"/>
       <c r="C467" s="2" t="inlineStr">
         <is>
-          <t>A0001140</t>
+          <t>PED-KEDADA</t>
         </is>
       </c>
       <c r="D467" s="2" t="inlineStr"/>
@@ -35075,7 +35075,7 @@
       <c r="B468" s="2" t="inlineStr"/>
       <c r="C468" s="2" t="inlineStr">
         <is>
-          <t>A0001141</t>
+          <t>PED-KEDADA-1</t>
         </is>
       </c>
       <c r="D468" s="2" t="inlineStr"/>
@@ -35149,7 +35149,7 @@
       <c r="B469" s="2" t="inlineStr"/>
       <c r="C469" s="2" t="inlineStr">
         <is>
-          <t>A0001142</t>
+          <t>PED-HOPEBA</t>
         </is>
       </c>
       <c r="D469" s="2" t="inlineStr"/>
@@ -35223,7 +35223,7 @@
       <c r="B470" s="2" t="inlineStr"/>
       <c r="C470" s="2" t="inlineStr">
         <is>
-          <t>A0001149</t>
+          <t>TC-IMTOCO-6</t>
         </is>
       </c>
       <c r="D470" s="2" t="inlineStr"/>
@@ -35297,7 +35297,7 @@
       <c r="B471" s="2" t="inlineStr"/>
       <c r="C471" s="2" t="inlineStr">
         <is>
-          <t>A0001152</t>
+          <t>TC-IMTOCO-7</t>
         </is>
       </c>
       <c r="D471" s="2" t="inlineStr"/>
@@ -35371,7 +35371,7 @@
       <c r="B472" s="2" t="inlineStr"/>
       <c r="C472" s="2" t="inlineStr">
         <is>
-          <t>A0001158</t>
+          <t>DUA-DULU60</t>
         </is>
       </c>
       <c r="D472" s="2" t="inlineStr"/>
@@ -35445,7 +35445,7 @@
       <c r="B473" s="2" t="inlineStr"/>
       <c r="C473" s="2" t="inlineStr">
         <is>
-          <t>A0001162</t>
+          <t>PED-TUNILO</t>
         </is>
       </c>
       <c r="D473" s="2" t="inlineStr"/>
@@ -35519,7 +35519,7 @@
       <c r="B474" s="2" t="inlineStr"/>
       <c r="C474" s="2" t="inlineStr">
         <is>
-          <t>A0001165</t>
+          <t>DD-DENOMI</t>
         </is>
       </c>
       <c r="D474" s="2" t="inlineStr"/>
@@ -35593,7 +35593,7 @@
       <c r="B475" s="2" t="inlineStr"/>
       <c r="C475" s="2" t="inlineStr">
         <is>
-          <t>A0001166</t>
+          <t>DD-DEBALE-1</t>
         </is>
       </c>
       <c r="D475" s="2" t="inlineStr"/>
@@ -35667,7 +35667,7 @@
       <c r="B476" s="2" t="inlineStr"/>
       <c r="C476" s="2" t="inlineStr">
         <is>
-          <t>A0001167</t>
+          <t>TIP-TILAMA</t>
         </is>
       </c>
       <c r="D476" s="2" t="inlineStr"/>
@@ -35741,7 +35741,7 @@
       <c r="B477" s="2" t="inlineStr"/>
       <c r="C477" s="2" t="inlineStr">
         <is>
-          <t>A0001169</t>
+          <t>PED-THCHCH</t>
         </is>
       </c>
       <c r="D477" s="2" t="inlineStr"/>
@@ -35815,7 +35815,7 @@
       <c r="B478" s="2" t="inlineStr"/>
       <c r="C478" s="2" t="inlineStr">
         <is>
-          <t>A0001170</t>
+          <t>TA-KIBAMO-1</t>
         </is>
       </c>
       <c r="D478" s="2" t="inlineStr"/>
@@ -35889,7 +35889,7 @@
       <c r="B479" s="2" t="inlineStr"/>
       <c r="C479" s="2" t="inlineStr">
         <is>
-          <t>A0001171</t>
+          <t>TIP-TITRTH</t>
         </is>
       </c>
       <c r="D479" s="2" t="inlineStr"/>
@@ -35963,7 +35963,7 @@
       <c r="B480" s="2" t="inlineStr"/>
       <c r="C480" s="2" t="inlineStr">
         <is>
-          <t>A0001172</t>
+          <t>TIP-TITHVU</t>
         </is>
       </c>
       <c r="D480" s="2" t="inlineStr"/>
@@ -36037,7 +36037,7 @@
       <c r="B481" s="2" t="inlineStr"/>
       <c r="C481" s="2" t="inlineStr">
         <is>
-          <t>A0001173</t>
+          <t>TIP-TITRNH-2</t>
         </is>
       </c>
       <c r="D481" s="2" t="inlineStr"/>
@@ -36111,7 +36111,7 @@
       <c r="B482" s="2" t="inlineStr"/>
       <c r="C482" s="2" t="inlineStr">
         <is>
-          <t>A0001174</t>
+          <t>TA-KITHDA</t>
         </is>
       </c>
       <c r="D482" s="2" t="inlineStr"/>
@@ -36185,7 +36185,7 @@
       <c r="B483" s="2" t="inlineStr"/>
       <c r="C483" s="2" t="inlineStr">
         <is>
-          <t>A0001175</t>
+          <t>BUT-BUCHBI</t>
         </is>
       </c>
       <c r="D483" s="2" t="inlineStr"/>
@@ -36259,7 +36259,7 @@
       <c r="B484" s="2" t="inlineStr"/>
       <c r="C484" s="2" t="inlineStr">
         <is>
-          <t>A0001177</t>
+          <t>DB-BAMI3I-2</t>
         </is>
       </c>
       <c r="D484" s="2" t="inlineStr"/>
@@ -36333,7 +36333,7 @@
       <c r="B485" s="2" t="inlineStr"/>
       <c r="C485" s="2" t="inlineStr">
         <is>
-          <t>A0001178</t>
+          <t>DB-BAMI5I</t>
         </is>
       </c>
       <c r="D485" s="2" t="inlineStr"/>
@@ -36407,7 +36407,7 @@
       <c r="B486" s="2" t="inlineStr"/>
       <c r="C486" s="2" t="inlineStr">
         <is>
-          <t>A0001179</t>
+          <t>DB-BAMIDI-1</t>
         </is>
       </c>
       <c r="D486" s="2" t="inlineStr"/>
@@ -36481,7 +36481,7 @@
       <c r="B487" s="2" t="inlineStr"/>
       <c r="C487" s="2" t="inlineStr">
         <is>
-          <t>A0001183</t>
+          <t>DD-DEHYSO</t>
         </is>
       </c>
       <c r="D487" s="2" t="inlineStr"/>
@@ -36555,7 +36555,7 @@
       <c r="B488" s="2" t="inlineStr"/>
       <c r="C488" s="2" t="inlineStr">
         <is>
-          <t>A0001184</t>
+          <t>TA-HOTRDU</t>
         </is>
       </c>
       <c r="D488" s="2" t="inlineStr"/>
@@ -36629,7 +36629,7 @@
       <c r="B489" s="2" t="inlineStr"/>
       <c r="C489" s="2" t="inlineStr">
         <is>
-          <t>A0001192</t>
+          <t>GD-GEDA</t>
         </is>
       </c>
       <c r="D489" s="2" t="inlineStr"/>
@@ -36703,7 +36703,7 @@
       <c r="B490" s="2" t="inlineStr"/>
       <c r="C490" s="2" t="inlineStr">
         <is>
-          <t>A0001193</t>
+          <t>GD-GEDA-1</t>
         </is>
       </c>
       <c r="D490" s="2" t="inlineStr"/>
@@ -36777,7 +36777,7 @@
       <c r="B491" s="2" t="inlineStr"/>
       <c r="C491" s="2" t="inlineStr">
         <is>
-          <t>A0001194</t>
+          <t>GD-GEDA-2</t>
         </is>
       </c>
       <c r="D491" s="2" t="inlineStr"/>
@@ -36851,7 +36851,7 @@
       <c r="B492" s="2" t="inlineStr"/>
       <c r="C492" s="2" t="inlineStr">
         <is>
-          <t>A0001195</t>
+          <t>GD-GEDA-3</t>
         </is>
       </c>
       <c r="D492" s="2" t="inlineStr"/>
@@ -36925,7 +36925,7 @@
       <c r="B493" s="2" t="inlineStr"/>
       <c r="C493" s="2" t="inlineStr">
         <is>
-          <t>A0001196</t>
+          <t>GD-GEDA-4</t>
         </is>
       </c>
       <c r="D493" s="2" t="inlineStr"/>
@@ -36999,7 +36999,7 @@
       <c r="B494" s="2" t="inlineStr"/>
       <c r="C494" s="2" t="inlineStr">
         <is>
-          <t>A0001197</t>
+          <t>GD-GEDA-5</t>
         </is>
       </c>
       <c r="D494" s="2" t="inlineStr"/>
@@ -37073,7 +37073,7 @@
       <c r="B495" s="2" t="inlineStr"/>
       <c r="C495" s="2" t="inlineStr">
         <is>
-          <t>A0001198</t>
+          <t>GD-GEDA-6</t>
         </is>
       </c>
       <c r="D495" s="2" t="inlineStr"/>
@@ -37147,7 +37147,7 @@
       <c r="B496" s="2" t="inlineStr"/>
       <c r="C496" s="2" t="inlineStr">
         <is>
-          <t>A0001199</t>
+          <t>GD-GEDA-7</t>
         </is>
       </c>
       <c r="D496" s="2" t="inlineStr"/>
@@ -37221,7 +37221,7 @@
       <c r="B497" s="2" t="inlineStr"/>
       <c r="C497" s="2" t="inlineStr">
         <is>
-          <t>A0001200</t>
+          <t>GD-GEDA-8</t>
         </is>
       </c>
       <c r="D497" s="2" t="inlineStr"/>
@@ -37295,7 +37295,7 @@
       <c r="B498" s="2" t="inlineStr"/>
       <c r="C498" s="2" t="inlineStr">
         <is>
-          <t>A0001201</t>
+          <t>GD-GEDA-9</t>
         </is>
       </c>
       <c r="D498" s="2" t="inlineStr"/>
@@ -37369,7 +37369,7 @@
       <c r="B499" s="2" t="inlineStr"/>
       <c r="C499" s="2" t="inlineStr">
         <is>
-          <t>A0001202</t>
+          <t>GD-GEDA-10</t>
         </is>
       </c>
       <c r="D499" s="2" t="inlineStr"/>
@@ -37443,7 +37443,7 @@
       <c r="B500" s="2" t="inlineStr"/>
       <c r="C500" s="2" t="inlineStr">
         <is>
-          <t>A0001203</t>
+          <t>GD-GEDA-11</t>
         </is>
       </c>
       <c r="D500" s="2" t="inlineStr"/>
@@ -37517,7 +37517,7 @@
       <c r="B501" s="2" t="inlineStr"/>
       <c r="C501" s="2" t="inlineStr">
         <is>
-          <t>A0001204</t>
+          <t>GD-GEDA-12</t>
         </is>
       </c>
       <c r="D501" s="2" t="inlineStr"/>
@@ -37591,7 +37591,7 @@
       <c r="B502" s="2" t="inlineStr"/>
       <c r="C502" s="2" t="inlineStr">
         <is>
-          <t>A0001205</t>
+          <t>GD-GEDA-13</t>
         </is>
       </c>
       <c r="D502" s="2" t="inlineStr"/>
@@ -37665,7 +37665,7 @@
       <c r="B503" s="2" t="inlineStr"/>
       <c r="C503" s="2" t="inlineStr">
         <is>
-          <t>A0001212</t>
+          <t>TC-CNSHBA</t>
         </is>
       </c>
       <c r="D503" s="2" t="inlineStr"/>
@@ -37739,7 +37739,7 @@
       <c r="B504" s="2" t="inlineStr"/>
       <c r="C504" s="2" t="inlineStr">
         <is>
-          <t>A0001213</t>
+          <t>HC-COXA80</t>
         </is>
       </c>
       <c r="D504" s="2" t="inlineStr"/>
@@ -37813,7 +37813,7 @@
       <c r="B505" s="2" t="inlineStr"/>
       <c r="C505" s="2" t="inlineStr">
         <is>
-          <t>A0001217</t>
+          <t>PED-TH5IPE</t>
         </is>
       </c>
       <c r="D505" s="2" t="inlineStr"/>
@@ -37887,7 +37887,7 @@
       <c r="B506" s="2" t="inlineStr"/>
       <c r="C506" s="2" t="inlineStr">
         <is>
-          <t>A0001220</t>
+          <t>HC-OIVIDU</t>
         </is>
       </c>
       <c r="D506" s="2" t="inlineStr"/>
@@ -37961,7 +37961,7 @@
       <c r="B507" s="2" t="inlineStr"/>
       <c r="C507" s="2" t="inlineStr">
         <is>
-          <t>A0001224</t>
+          <t>NOE-HOCUOI</t>
         </is>
       </c>
       <c r="D507" s="2" t="inlineStr"/>
@@ -38035,7 +38035,7 @@
       <c r="B508" s="2" t="inlineStr"/>
       <c r="C508" s="2" t="inlineStr">
         <is>
-          <t>A0001225</t>
+          <t>NOE-CUOINO</t>
         </is>
       </c>
       <c r="D508" s="2" t="inlineStr"/>
@@ -38109,7 +38109,7 @@
       <c r="B509" s="2" t="inlineStr"/>
       <c r="C509" s="2" t="inlineStr">
         <is>
-          <t>A0001226</t>
+          <t>NOE-KEHODO</t>
         </is>
       </c>
       <c r="D509" s="2" t="inlineStr"/>
@@ -38183,7 +38183,7 @@
       <c r="B510" s="2" t="inlineStr"/>
       <c r="C510" s="2" t="inlineStr">
         <is>
-          <t>A0001227</t>
+          <t>NOE-HOKEMA</t>
         </is>
       </c>
       <c r="D510" s="2" t="inlineStr"/>
@@ -38257,7 +38257,7 @@
       <c r="B511" s="2" t="inlineStr"/>
       <c r="C511" s="2" t="inlineStr">
         <is>
-          <t>A0001229</t>
+          <t>PED-DAMA</t>
         </is>
       </c>
       <c r="D511" s="2" t="inlineStr"/>
@@ -38331,7 +38331,7 @@
       <c r="B512" s="2" t="inlineStr"/>
       <c r="C512" s="2" t="inlineStr">
         <is>
-          <t>A0001232</t>
+          <t>BOT-BOOMNU</t>
         </is>
       </c>
       <c r="D512" s="2" t="inlineStr"/>
@@ -38405,7 +38405,7 @@
       <c r="B513" s="2" t="inlineStr"/>
       <c r="C513" s="2" t="inlineStr">
         <is>
-          <t>A0001238</t>
+          <t>BOT-BOOM-2</t>
         </is>
       </c>
       <c r="D513" s="2" t="inlineStr"/>

</xml_diff>